<commit_message>
commit to go with Erudite v1.1.0 release
</commit_message>
<xml_diff>
--- a/AFootball testing results.xlsx
+++ b/AFootball testing results.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Season results" sheetId="1" r:id="rId1"/>
     <sheet name="Week 4 results" sheetId="2" r:id="rId2"/>
     <sheet name="Week 5 results" sheetId="3" r:id="rId3"/>
     <sheet name="Week 6 results" sheetId="4" r:id="rId4"/>
+    <sheet name="Week 7 results" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="239">
   <si>
     <t>AF613_logsig base randomized w&amp;b*</t>
   </si>
@@ -1376,6 +1377,69 @@
   </si>
   <si>
     <t>ON001(home win): 0.9999 / ON002(away win): 6.8e-11</t>
+  </si>
+  <si>
+    <t>AFNNET_12-8-2_logsig</t>
+  </si>
+  <si>
+    <t>AFNNET_18H2L_logsig</t>
+  </si>
+  <si>
+    <t>AFNNET_12H2L_logsig</t>
+  </si>
+  <si>
+    <t>AFNNET_6H1Lv2_logsig</t>
+  </si>
+  <si>
+    <t>AFNNET_6H1L_logsig</t>
+  </si>
+  <si>
+    <t>AFNNET_logsig base rand</t>
+  </si>
+  <si>
+    <t>SEA(a) @ ARI(h) 2013 week 7</t>
+  </si>
+  <si>
+    <t>SD(a) @ JAC(h) 2013 week 7</t>
+  </si>
+  <si>
+    <t>CIN(a) @ DET(h) 2013 week 7</t>
+  </si>
+  <si>
+    <t>BUF(a) @ MIA(h) 2013 week 7</t>
+  </si>
+  <si>
+    <t>TB(a) @ ATL(h) 2013 week 7</t>
+  </si>
+  <si>
+    <t>NE(a) @ NYJ(h) 2013 week 7</t>
+  </si>
+  <si>
+    <t>DAL(a) @ PHI(h) 2013 week 7</t>
+  </si>
+  <si>
+    <t>CHI(a) @ WAS(h) 2013 week 7</t>
+  </si>
+  <si>
+    <t>STL(a) @ CAR(h) 2013 week 7</t>
+  </si>
+  <si>
+    <t>SF(a) @ TEN(h) 2013 week 7</t>
+  </si>
+  <si>
+    <t>CLE(a) @ GB(h) 2013 week 7</t>
+  </si>
+  <si>
+    <t>HOU(a) @ KC(h) 2013 week 7</t>
+  </si>
+  <si>
+    <t>BAL(a) @ PIT(h) 2013 week 7</t>
+  </si>
+  <si>
+    <t>DEN(a) @ IND(h) 2013 week 7</t>
+  </si>
+  <si>
+    <t>MIN(a) @ NYG(h) 2013 week 7</t>
   </si>
 </sst>
 </file>
@@ -1489,7 +1553,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1519,6 +1583,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1880,8 +1947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1918,8 +1985,8 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
+      <c r="A2" s="15" t="s">
+        <v>223</v>
       </c>
       <c r="B2">
         <f>'Week 4 results'!B2+'Week 5 results'!B2+'Week 6 results'!B2</f>
@@ -1938,17 +2005,17 @@
         <v>31</v>
       </c>
       <c r="F2" s="14">
-        <f>B2/(E2-D2)</f>
+        <f t="shared" ref="F2:F7" si="1">B2/(E2-D2)</f>
         <v>0.6</v>
       </c>
       <c r="G2" s="14">
-        <f>B2/E2</f>
+        <f t="shared" ref="G2:G7" si="2">B2/E2</f>
         <v>0.58064516129032262</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
+      <c r="A3" t="s">
+        <v>222</v>
       </c>
       <c r="B3">
         <f>'Week 4 results'!B3+'Week 5 results'!B3+'Week 6 results'!B3</f>
@@ -1967,17 +2034,17 @@
         <v>31</v>
       </c>
       <c r="F3" s="14">
-        <f>B3/(E3-D3)</f>
+        <f t="shared" si="1"/>
         <v>0.62068965517241381</v>
       </c>
       <c r="G3" s="14">
-        <f>B3/E3</f>
+        <f t="shared" si="2"/>
         <v>0.58064516129032262</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
+      <c r="A4" t="s">
+        <v>221</v>
       </c>
       <c r="B4">
         <f>'Week 4 results'!B4+'Week 5 results'!B4+'Week 6 results'!B4</f>
@@ -1996,17 +2063,17 @@
         <v>31</v>
       </c>
       <c r="F4" s="14">
-        <f>B4/(E4-D4)</f>
+        <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
       <c r="G4" s="14">
-        <f>B4/E4</f>
+        <f t="shared" si="2"/>
         <v>0.67741935483870963</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
+      <c r="A5" t="s">
+        <v>220</v>
       </c>
       <c r="B5">
         <f>'Week 4 results'!B5+'Week 5 results'!B5+'Week 6 results'!B5</f>
@@ -2025,17 +2092,17 @@
         <v>31</v>
       </c>
       <c r="F5" s="14">
-        <f>B5/(E5-D5)</f>
+        <f t="shared" si="1"/>
         <v>0.70370370370370372</v>
       </c>
       <c r="G5" s="14">
-        <f>B5/E5</f>
+        <f t="shared" si="2"/>
         <v>0.61290322580645162</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
+      <c r="A6" t="s">
+        <v>219</v>
       </c>
       <c r="B6">
         <f>'Week 4 results'!B6+'Week 5 results'!B6+'Week 6 results'!B6</f>
@@ -2054,17 +2121,17 @@
         <v>31</v>
       </c>
       <c r="F6" s="14">
-        <f>B6/(E6-D6)</f>
+        <f t="shared" si="1"/>
         <v>0.6071428571428571</v>
       </c>
       <c r="G6" s="14">
-        <f>B6/E6</f>
+        <f t="shared" si="2"/>
         <v>0.54838709677419351</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="3" t="s">
-        <v>5</v>
+      <c r="A7" t="s">
+        <v>218</v>
       </c>
       <c r="B7">
         <f>'Week 4 results'!B7+'Week 5 results'!B7+'Week 6 results'!B7</f>
@@ -2083,11 +2150,11 @@
         <v>31</v>
       </c>
       <c r="F7" s="14">
-        <f>B7/(E7-D7)</f>
+        <f t="shared" si="1"/>
         <v>0.56666666666666665</v>
       </c>
       <c r="G7" s="14">
-        <f>B7/E7</f>
+        <f t="shared" si="2"/>
         <v>0.54838709677419351</v>
       </c>
     </row>
@@ -2700,7 +2767,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2"/>
+      <selection pane="topRight" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3127,4 +3194,112 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:S7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="5" max="19" width="51.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
testing results spreadsheet update for wk. 7
</commit_message>
<xml_diff>
--- a/AFootball testing results.xlsx
+++ b/AFootball testing results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Season results" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="251">
   <si>
     <t>AF613_logsig base randomized w&amp;b*</t>
   </si>
@@ -1397,9 +1397,6 @@
     <t>AFNNET_logsig base rand</t>
   </si>
   <si>
-    <t>SEA(a) @ ARI(h) 2013 week 7</t>
-  </si>
-  <si>
     <t>SD(a) @ JAC(h) 2013 week 7</t>
   </si>
   <si>
@@ -1440,6 +1437,66 @@
   </si>
   <si>
     <t>MIN(a) @ NYG(h) 2013 week 7</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SEA(a)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> @ ARI(h) 2013 week 7</t>
+    </r>
+  </si>
+  <si>
+    <t>ON001(home win): 0.0017 / ON002(away win): 0.9982</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.7606 / ON002(away win): 0.2393</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9703 / ON002(away win): 0.0296</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.1607 / ON002(away win): 0.8392</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.1412 / ON002(away win): 0.8587</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.0021 / ON002(away win): 0.9978</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9997 / ON002(away win): 0.0002</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.0118 / ON002(away win): 0.9881</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9695 / ON002(away win): 0.0304</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.7443 / ON002(away win): 0.2556</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.0857 / ON002(away win): 0.9142</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.0751 / ON002(away win): 0.9248</t>
   </si>
 </sst>
 </file>
@@ -1948,7 +2005,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1989,15 +2046,15 @@
         <v>223</v>
       </c>
       <c r="B2">
-        <f>'Week 4 results'!B2+'Week 5 results'!B2+'Week 6 results'!B2</f>
+        <f>'Week 4 results'!B2+'Week 5 results'!B2+'Week 6 results'!B2+'Week 7 results'!B2</f>
         <v>18</v>
       </c>
       <c r="C2">
-        <f>'Week 4 results'!C2+'Week 5 results'!C2+'Week 6 results'!C2</f>
+        <f>'Week 4 results'!C2+'Week 5 results'!C2+'Week 6 results'!C2+'Week 7 results'!C2</f>
         <v>12</v>
       </c>
       <c r="D2">
-        <f>'Week 4 results'!D2+'Week 5 results'!D2+'Week 6 results'!D2</f>
+        <f>'Week 4 results'!D2+'Week 5 results'!D2+'Week 6 results'!D2+'Week 7 results'!D2</f>
         <v>1</v>
       </c>
       <c r="E2">
@@ -2018,15 +2075,15 @@
         <v>222</v>
       </c>
       <c r="B3">
-        <f>'Week 4 results'!B3+'Week 5 results'!B3+'Week 6 results'!B3</f>
+        <f>'Week 4 results'!B3+'Week 5 results'!B3+'Week 6 results'!B3+'Week 7 results'!B3</f>
         <v>18</v>
       </c>
       <c r="C3">
-        <f>'Week 4 results'!C3+'Week 5 results'!C3+'Week 6 results'!C3</f>
+        <f>'Week 4 results'!C3+'Week 5 results'!C3+'Week 6 results'!C3+'Week 7 results'!C3</f>
         <v>11</v>
       </c>
       <c r="D3">
-        <f>'Week 4 results'!D3+'Week 5 results'!D3+'Week 6 results'!D3</f>
+        <f>'Week 4 results'!D3+'Week 5 results'!D3+'Week 6 results'!D3+'Week 7 results'!D3</f>
         <v>2</v>
       </c>
       <c r="E3">
@@ -2047,28 +2104,28 @@
         <v>221</v>
       </c>
       <c r="B4">
-        <f>'Week 4 results'!B4+'Week 5 results'!B4+'Week 6 results'!B4</f>
-        <v>21</v>
+        <f>'Week 4 results'!B4+'Week 5 results'!B4+'Week 6 results'!B4+'Week 7 results'!B4</f>
+        <v>22</v>
       </c>
       <c r="C4">
-        <f>'Week 4 results'!C4+'Week 5 results'!C4+'Week 6 results'!C4</f>
+        <f>'Week 4 results'!C4+'Week 5 results'!C4+'Week 6 results'!C4+'Week 7 results'!C4</f>
         <v>9</v>
       </c>
       <c r="D4">
-        <f>'Week 4 results'!D4+'Week 5 results'!D4+'Week 6 results'!D4</f>
+        <f>'Week 4 results'!D4+'Week 5 results'!D4+'Week 6 results'!D4+'Week 7 results'!D4</f>
         <v>1</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F4" s="14">
         <f t="shared" si="1"/>
-        <v>0.7</v>
+        <v>0.70967741935483875</v>
       </c>
       <c r="G4" s="14">
         <f t="shared" si="2"/>
-        <v>0.67741935483870963</v>
+        <v>0.6875</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2076,19 +2133,19 @@
         <v>220</v>
       </c>
       <c r="B5">
-        <f>'Week 4 results'!B5+'Week 5 results'!B5+'Week 6 results'!B5</f>
+        <f>'Week 4 results'!B5+'Week 5 results'!B5+'Week 6 results'!B5+'Week 7 results'!B5</f>
         <v>19</v>
       </c>
       <c r="C5">
-        <f>'Week 4 results'!C5+'Week 5 results'!C5+'Week 6 results'!C5</f>
+        <f>'Week 4 results'!C5+'Week 5 results'!C5+'Week 6 results'!C5+'Week 7 results'!C5</f>
         <v>8</v>
       </c>
       <c r="D5">
-        <f>'Week 4 results'!D5+'Week 5 results'!D5+'Week 6 results'!D5</f>
+        <f>'Week 4 results'!D5+'Week 5 results'!D5+'Week 6 results'!D5+'Week 7 results'!D5</f>
         <v>4</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f>B5+C5+D5</f>
         <v>31</v>
       </c>
       <c r="F5" s="14">
@@ -2105,15 +2162,15 @@
         <v>219</v>
       </c>
       <c r="B6">
-        <f>'Week 4 results'!B6+'Week 5 results'!B6+'Week 6 results'!B6</f>
+        <f>'Week 4 results'!B6+'Week 5 results'!B6+'Week 6 results'!B6+'Week 7 results'!B6</f>
         <v>17</v>
       </c>
       <c r="C6">
-        <f>'Week 4 results'!C6+'Week 5 results'!C6+'Week 6 results'!C6</f>
+        <f>'Week 4 results'!C6+'Week 5 results'!C6+'Week 6 results'!C6+'Week 7 results'!C6</f>
         <v>11</v>
       </c>
       <c r="D6">
-        <f>'Week 4 results'!D6+'Week 5 results'!D6+'Week 6 results'!D6</f>
+        <f>'Week 4 results'!D6+'Week 5 results'!D6+'Week 6 results'!D6+'Week 7 results'!D6</f>
         <v>3</v>
       </c>
       <c r="E6">
@@ -2134,15 +2191,15 @@
         <v>218</v>
       </c>
       <c r="B7">
-        <f>'Week 4 results'!B7+'Week 5 results'!B7+'Week 6 results'!B7</f>
+        <f>'Week 4 results'!B7+'Week 5 results'!B7+'Week 6 results'!B7+'Week 7 results'!B7</f>
         <v>17</v>
       </c>
       <c r="C7">
-        <f>'Week 4 results'!C7+'Week 5 results'!C7+'Week 6 results'!C7</f>
+        <f>'Week 4 results'!C7+'Week 5 results'!C7+'Week 6 results'!C7+'Week 7 results'!C6</f>
         <v>13</v>
       </c>
       <c r="D7">
-        <f>'Week 4 results'!D7+'Week 5 results'!D7+'Week 6 results'!D7</f>
+        <f>'Week 4 results'!D7+'Week 5 results'!D7+'Week 6 results'!D7+'Week 7 results'!D7</f>
         <v>1</v>
       </c>
       <c r="E7">
@@ -2168,8 +2225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2767,7 +2824,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:XFD1"/>
+      <selection pane="topRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3200,8 +3257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3224,82 +3281,182 @@
         <v>187</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>237</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" t="s">
+        <v>239</v>
+      </c>
+      <c r="H4" t="s">
+        <v>240</v>
+      </c>
+      <c r="I4" t="s">
+        <v>241</v>
+      </c>
+      <c r="J4" t="s">
+        <v>242</v>
+      </c>
+      <c r="K4" t="s">
+        <v>243</v>
+      </c>
+      <c r="L4" t="s">
+        <v>244</v>
+      </c>
+      <c r="M4" t="s">
+        <v>245</v>
+      </c>
+      <c r="N4" t="s">
+        <v>246</v>
+      </c>
+      <c r="O4" t="s">
+        <v>247</v>
+      </c>
+      <c r="P4" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>248</v>
+      </c>
+      <c r="R4" t="s">
+        <v>249</v>
+      </c>
+      <c r="S4" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
testing_results spreadsheet update week 7
</commit_message>
<xml_diff>
--- a/AFootball testing results.xlsx
+++ b/AFootball testing results.xlsx
@@ -1397,30 +1397,6 @@
     <t>AFNNET_logsig base rand</t>
   </si>
   <si>
-    <t>SD(a) @ JAC(h) 2013 week 7</t>
-  </si>
-  <si>
-    <t>CIN(a) @ DET(h) 2013 week 7</t>
-  </si>
-  <si>
-    <t>BUF(a) @ MIA(h) 2013 week 7</t>
-  </si>
-  <si>
-    <t>TB(a) @ ATL(h) 2013 week 7</t>
-  </si>
-  <si>
-    <t>NE(a) @ NYJ(h) 2013 week 7</t>
-  </si>
-  <si>
-    <t>DAL(a) @ PHI(h) 2013 week 7</t>
-  </si>
-  <si>
-    <t>CHI(a) @ WAS(h) 2013 week 7</t>
-  </si>
-  <si>
-    <t>STL(a) @ CAR(h) 2013 week 7</t>
-  </si>
-  <si>
     <t>SF(a) @ TEN(h) 2013 week 7</t>
   </si>
   <si>
@@ -1698,6 +1674,210 @@
   </si>
   <si>
     <t>ON001(home win): 0.0013 / ON002(away win): 0.9984</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SD(a)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> @ JAC(h) 2013 week 7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CIN(a)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> @ DET(h) 2013 week 7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BUF(a)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> @ MIA(h) 2013 week 7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">TB(a) @ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ATL(h)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2013 week 7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">NE(a) @ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NYJ(h)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2013 week 7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DAL(a)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> @ PHI(h) 2013 week 7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CHI(a) @ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WAS(h)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2013 week 7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">STL(a) @ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CAR(h)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2013 week 7</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2248,11 +2428,11 @@
       </c>
       <c r="B2">
         <f>'Week 4 results'!B2+'Week 5 results'!B2+'Week 6 results'!B2+'Week 7 results'!B2</f>
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C2">
         <f>'Week 4 results'!C2+'Week 5 results'!C2+'Week 6 results'!C2+'Week 7 results'!C2</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D2">
         <f>'Week 4 results'!D2+'Week 5 results'!D2+'Week 6 results'!D2+'Week 7 results'!D2</f>
@@ -2260,15 +2440,15 @@
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E7" si="0">B2+C2+D2</f>
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="F2" s="14">
         <f t="shared" ref="F2:F7" si="1">B2/(E2-D2)</f>
-        <v>0.61290322580645162</v>
+        <v>0.58974358974358976</v>
       </c>
       <c r="G2" s="14">
         <f t="shared" ref="G2:G7" si="2">B2/E2</f>
-        <v>0.59375</v>
+        <v>0.57499999999999996</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2277,11 +2457,11 @@
       </c>
       <c r="B3">
         <f>'Week 4 results'!B3+'Week 5 results'!B3+'Week 6 results'!B3+'Week 7 results'!B3</f>
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C3">
         <f>'Week 4 results'!C3+'Week 5 results'!C3+'Week 6 results'!C3+'Week 7 results'!C3</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D3">
         <f>'Week 4 results'!D3+'Week 5 results'!D3+'Week 6 results'!D3+'Week 7 results'!D3</f>
@@ -2289,15 +2469,15 @@
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="F3" s="14">
         <f t="shared" si="1"/>
-        <v>0.6333333333333333</v>
+        <v>0.6216216216216216</v>
       </c>
       <c r="G3" s="14">
         <f t="shared" si="2"/>
-        <v>0.5757575757575758</v>
+        <v>0.57499999999999996</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2306,11 +2486,11 @@
       </c>
       <c r="B4">
         <f>'Week 4 results'!B4+'Week 5 results'!B4+'Week 6 results'!B4+'Week 7 results'!B4</f>
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C4">
         <f>'Week 4 results'!C4+'Week 5 results'!C4+'Week 6 results'!C4+'Week 7 results'!C4</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D4">
         <f>'Week 4 results'!D4+'Week 5 results'!D4+'Week 6 results'!D4+'Week 7 results'!D4</f>
@@ -2318,15 +2498,15 @@
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="F4" s="14">
         <f t="shared" si="1"/>
-        <v>0.70967741935483875</v>
+        <v>0.69230769230769229</v>
       </c>
       <c r="G4" s="14">
         <f t="shared" si="2"/>
-        <v>0.6875</v>
+        <v>0.67500000000000004</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2335,11 +2515,11 @@
       </c>
       <c r="B5">
         <f>'Week 4 results'!B5+'Week 5 results'!B5+'Week 6 results'!B5+'Week 7 results'!B5</f>
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C5">
         <f>'Week 4 results'!C5+'Week 5 results'!C5+'Week 6 results'!C5+'Week 7 results'!C5</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <f>'Week 4 results'!D5+'Week 5 results'!D5+'Week 6 results'!D5+'Week 7 results'!D5</f>
@@ -2347,15 +2527,15 @@
       </c>
       <c r="E5">
         <f>B5+C5+D5</f>
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="F5" s="14">
         <f t="shared" si="1"/>
-        <v>0.7142857142857143</v>
+        <v>0.67647058823529416</v>
       </c>
       <c r="G5" s="14">
         <f t="shared" si="2"/>
-        <v>0.58823529411764708</v>
+        <v>0.57499999999999996</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2364,11 +2544,11 @@
       </c>
       <c r="B6">
         <f>'Week 4 results'!B6+'Week 5 results'!B6+'Week 6 results'!B6+'Week 7 results'!B6</f>
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C6">
         <f>'Week 4 results'!C6+'Week 5 results'!C6+'Week 6 results'!C6+'Week 7 results'!C6</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D6">
         <f>'Week 4 results'!D6+'Week 5 results'!D6+'Week 6 results'!D6+'Week 7 results'!D6</f>
@@ -2376,15 +2556,15 @@
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="F6" s="14">
         <f t="shared" si="1"/>
-        <v>0.62068965517241381</v>
+        <v>0.61111111111111116</v>
       </c>
       <c r="G6" s="14">
         <f t="shared" si="2"/>
-        <v>0.54545454545454541</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2393,11 +2573,11 @@
       </c>
       <c r="B7">
         <f>'Week 4 results'!B7+'Week 5 results'!B7+'Week 6 results'!B7+'Week 7 results'!B7</f>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C7">
         <f>'Week 4 results'!C7+'Week 5 results'!C7+'Week 6 results'!C7+'Week 7 results'!C6</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <f>'Week 4 results'!D7+'Week 5 results'!D7+'Week 6 results'!D7+'Week 7 results'!D7</f>
@@ -2405,15 +2585,15 @@
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="F7" s="14">
         <f t="shared" si="1"/>
-        <v>0.58064516129032262</v>
+        <v>0.58974358974358976</v>
       </c>
       <c r="G7" s="14">
         <f t="shared" si="2"/>
-        <v>0.5625</v>
+        <v>0.57499999999999996</v>
       </c>
     </row>
   </sheetData>
@@ -3459,7 +3639,7 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3482,49 +3662,49 @@
         <v>187</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>229</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -3532,58 +3712,58 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="N2" t="s">
+        <v>250</v>
+      </c>
+      <c r="O2" t="s">
         <v>251</v>
       </c>
-      <c r="F2" t="s">
+      <c r="P2" t="s">
         <v>252</v>
       </c>
-      <c r="G2" t="s">
+      <c r="Q2" t="s">
         <v>253</v>
       </c>
-      <c r="H2" t="s">
-        <v>172</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="R2" t="s">
         <v>254</v>
       </c>
-      <c r="J2" t="s">
+      <c r="S2" t="s">
         <v>255</v>
-      </c>
-      <c r="K2" t="s">
-        <v>256</v>
-      </c>
-      <c r="L2" t="s">
-        <v>73</v>
-      </c>
-      <c r="M2" t="s">
-        <v>257</v>
-      </c>
-      <c r="N2" t="s">
-        <v>258</v>
-      </c>
-      <c r="O2" t="s">
-        <v>259</v>
-      </c>
-      <c r="P2" t="s">
-        <v>260</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>261</v>
-      </c>
-      <c r="R2" t="s">
-        <v>262</v>
-      </c>
-      <c r="S2" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -3591,10 +3771,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -3602,47 +3782,47 @@
       <c r="E3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="N3" t="s">
         <v>291</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="O3" t="s">
         <v>292</v>
       </c>
-      <c r="H3" t="s">
+      <c r="P3" t="s">
         <v>293</v>
       </c>
-      <c r="I3" t="s">
+      <c r="Q3" t="s">
         <v>294</v>
       </c>
-      <c r="J3" t="s">
+      <c r="R3" t="s">
         <v>295</v>
       </c>
-      <c r="K3" t="s">
+      <c r="S3" t="s">
         <v>296</v>
-      </c>
-      <c r="L3" t="s">
-        <v>297</v>
-      </c>
-      <c r="M3" t="s">
-        <v>298</v>
-      </c>
-      <c r="N3" t="s">
-        <v>299</v>
-      </c>
-      <c r="O3" t="s">
-        <v>300</v>
-      </c>
-      <c r="P3" t="s">
-        <v>301</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>302</v>
-      </c>
-      <c r="R3" t="s">
-        <v>303</v>
-      </c>
-      <c r="S3" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -3650,10 +3830,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -3661,47 +3841,47 @@
       <c r="E4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="N4" t="s">
+        <v>238</v>
+      </c>
+      <c r="O4" t="s">
         <v>239</v>
-      </c>
-      <c r="H4" t="s">
-        <v>240</v>
-      </c>
-      <c r="I4" t="s">
-        <v>241</v>
-      </c>
-      <c r="J4" t="s">
-        <v>242</v>
-      </c>
-      <c r="K4" t="s">
-        <v>243</v>
-      </c>
-      <c r="L4" t="s">
-        <v>244</v>
-      </c>
-      <c r="M4" t="s">
-        <v>245</v>
-      </c>
-      <c r="N4" t="s">
-        <v>246</v>
-      </c>
-      <c r="O4" t="s">
-        <v>247</v>
       </c>
       <c r="P4" t="s">
         <v>172</v>
       </c>
       <c r="Q4" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="R4" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="S4" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -3709,58 +3889,58 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="M5" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="F5" t="s">
+      <c r="N5" t="s">
         <v>277</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="O5" t="s">
         <v>278</v>
       </c>
-      <c r="H5" t="s">
+      <c r="P5" t="s">
         <v>279</v>
       </c>
-      <c r="I5" t="s">
+      <c r="Q5" t="s">
         <v>280</v>
       </c>
-      <c r="J5" t="s">
+      <c r="R5" t="s">
         <v>281</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="S5" t="s">
         <v>282</v>
-      </c>
-      <c r="L5" t="s">
-        <v>283</v>
-      </c>
-      <c r="M5" t="s">
-        <v>284</v>
-      </c>
-      <c r="N5" t="s">
-        <v>285</v>
-      </c>
-      <c r="O5" t="s">
-        <v>286</v>
-      </c>
-      <c r="P5" t="s">
-        <v>287</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>288</v>
-      </c>
-      <c r="R5" t="s">
-        <v>289</v>
-      </c>
-      <c r="S5" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -3768,58 +3948,58 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6" t="s">
         <v>305</v>
-      </c>
-      <c r="F6" t="s">
-        <v>306</v>
-      </c>
-      <c r="G6" t="s">
-        <v>307</v>
-      </c>
-      <c r="H6" t="s">
-        <v>308</v>
-      </c>
-      <c r="I6" t="s">
-        <v>309</v>
-      </c>
-      <c r="J6" t="s">
-        <v>310</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>311</v>
-      </c>
-      <c r="L6" t="s">
-        <v>312</v>
-      </c>
-      <c r="M6" t="s">
-        <v>12</v>
-      </c>
-      <c r="N6" t="s">
-        <v>313</v>
       </c>
       <c r="O6" t="s">
         <v>116</v>
       </c>
       <c r="P6" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="Q6" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="R6" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="S6" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -3827,62 +4007,62 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="N7" t="s">
+        <v>262</v>
+      </c>
+      <c r="O7" t="s">
+        <v>263</v>
+      </c>
+      <c r="P7" t="s">
         <v>264</v>
       </c>
-      <c r="F7" t="s">
-        <v>264</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="Q7" t="s">
         <v>265</v>
       </c>
-      <c r="H7" t="s">
-        <v>105</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="R7" t="s">
         <v>266</v>
       </c>
-      <c r="J7" t="s">
+      <c r="S7" t="s">
         <v>267</v>
-      </c>
-      <c r="K7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L7" t="s">
-        <v>268</v>
-      </c>
-      <c r="M7" t="s">
-        <v>269</v>
-      </c>
-      <c r="N7" t="s">
-        <v>270</v>
-      </c>
-      <c r="O7" t="s">
-        <v>271</v>
-      </c>
-      <c r="P7" t="s">
-        <v>272</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>273</v>
-      </c>
-      <c r="R7" t="s">
-        <v>274</v>
-      </c>
-      <c r="S7" t="s">
-        <v>275</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Testing results spreadsheet update
Week 7 through sunday night
</commit_message>
<xml_diff>
--- a/AFootball testing results.xlsx
+++ b/AFootball testing results.xlsx
@@ -1397,21 +1397,6 @@
     <t>AFNNET_logsig base rand</t>
   </si>
   <si>
-    <t>SF(a) @ TEN(h) 2013 week 7</t>
-  </si>
-  <si>
-    <t>CLE(a) @ GB(h) 2013 week 7</t>
-  </si>
-  <si>
-    <t>HOU(a) @ KC(h) 2013 week 7</t>
-  </si>
-  <si>
-    <t>BAL(a) @ PIT(h) 2013 week 7</t>
-  </si>
-  <si>
-    <t>DEN(a) @ IND(h) 2013 week 7</t>
-  </si>
-  <si>
     <t>MIN(a) @ NYG(h) 2013 week 7</t>
   </si>
   <si>
@@ -1866,6 +1851,138 @@
         <scheme val="minor"/>
       </rPr>
       <t>CAR(h)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2013 week 7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SF(a)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> @ TEN(h) 2013 week 7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CLE(a) @ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GB(h)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2013 week 7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">HOU(a) @ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KC(h)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2013 week 7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">BAL(a) @ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PIT(h)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2013 week 7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">DEN(a) @ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IND(h)</t>
     </r>
     <r>
       <rPr>
@@ -2428,11 +2545,11 @@
       </c>
       <c r="B2">
         <f>'Week 4 results'!B2+'Week 5 results'!B2+'Week 6 results'!B2+'Week 7 results'!B2</f>
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C2">
         <f>'Week 4 results'!C2+'Week 5 results'!C2+'Week 6 results'!C2+'Week 7 results'!C2</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D2">
         <f>'Week 4 results'!D2+'Week 5 results'!D2+'Week 6 results'!D2+'Week 7 results'!D2</f>
@@ -2440,15 +2557,15 @@
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E7" si="0">B2+C2+D2</f>
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F2" s="14">
         <f t="shared" ref="F2:F7" si="1">B2/(E2-D2)</f>
-        <v>0.58974358974358976</v>
+        <v>0.59090909090909094</v>
       </c>
       <c r="G2" s="14">
         <f t="shared" ref="G2:G7" si="2">B2/E2</f>
-        <v>0.57499999999999996</v>
+        <v>0.57777777777777772</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2457,11 +2574,11 @@
       </c>
       <c r="B3">
         <f>'Week 4 results'!B3+'Week 5 results'!B3+'Week 6 results'!B3+'Week 7 results'!B3</f>
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <f>'Week 4 results'!C3+'Week 5 results'!C3+'Week 6 results'!C3+'Week 7 results'!C3</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3">
         <f>'Week 4 results'!D3+'Week 5 results'!D3+'Week 6 results'!D3+'Week 7 results'!D3</f>
@@ -2469,15 +2586,15 @@
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F3" s="14">
         <f t="shared" si="1"/>
-        <v>0.6216216216216216</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="G3" s="14">
         <f t="shared" si="2"/>
-        <v>0.57499999999999996</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2486,11 +2603,11 @@
       </c>
       <c r="B4">
         <f>'Week 4 results'!B4+'Week 5 results'!B4+'Week 6 results'!B4+'Week 7 results'!B4</f>
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C4">
         <f>'Week 4 results'!C4+'Week 5 results'!C4+'Week 6 results'!C4+'Week 7 results'!C4</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <f>'Week 4 results'!D4+'Week 5 results'!D4+'Week 6 results'!D4+'Week 7 results'!D4</f>
@@ -2498,15 +2615,15 @@
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F4" s="14">
         <f t="shared" si="1"/>
-        <v>0.69230769230769229</v>
+        <v>0.70454545454545459</v>
       </c>
       <c r="G4" s="14">
         <f t="shared" si="2"/>
-        <v>0.67500000000000004</v>
+        <v>0.68888888888888888</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2515,11 +2632,11 @@
       </c>
       <c r="B5">
         <f>'Week 4 results'!B5+'Week 5 results'!B5+'Week 6 results'!B5+'Week 7 results'!B5</f>
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C5">
         <f>'Week 4 results'!C5+'Week 5 results'!C5+'Week 6 results'!C5+'Week 7 results'!C5</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <f>'Week 4 results'!D5+'Week 5 results'!D5+'Week 6 results'!D5+'Week 7 results'!D5</f>
@@ -2527,15 +2644,15 @@
       </c>
       <c r="E5">
         <f>B5+C5+D5</f>
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F5" s="14">
         <f t="shared" si="1"/>
-        <v>0.67647058823529416</v>
+        <v>0.69230769230769229</v>
       </c>
       <c r="G5" s="14">
         <f t="shared" si="2"/>
-        <v>0.57499999999999996</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2544,11 +2661,11 @@
       </c>
       <c r="B6">
         <f>'Week 4 results'!B6+'Week 5 results'!B6+'Week 6 results'!B6+'Week 7 results'!B6</f>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C6">
         <f>'Week 4 results'!C6+'Week 5 results'!C6+'Week 6 results'!C6+'Week 7 results'!C6</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D6">
         <f>'Week 4 results'!D6+'Week 5 results'!D6+'Week 6 results'!D6+'Week 7 results'!D6</f>
@@ -2556,15 +2673,15 @@
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F6" s="14">
         <f t="shared" si="1"/>
-        <v>0.61111111111111116</v>
+        <v>0.6097560975609756</v>
       </c>
       <c r="G6" s="14">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.55555555555555558</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2573,11 +2690,11 @@
       </c>
       <c r="B7">
         <f>'Week 4 results'!B7+'Week 5 results'!B7+'Week 6 results'!B7+'Week 7 results'!B7</f>
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C7">
         <f>'Week 4 results'!C7+'Week 5 results'!C7+'Week 6 results'!C7+'Week 7 results'!C6</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D7">
         <f>'Week 4 results'!D7+'Week 5 results'!D7+'Week 6 results'!D7+'Week 7 results'!D7</f>
@@ -2585,15 +2702,15 @@
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F7" s="14">
         <f t="shared" si="1"/>
-        <v>0.58974358974358976</v>
+        <v>0.59090909090909094</v>
       </c>
       <c r="G7" s="14">
         <f t="shared" si="2"/>
-        <v>0.57499999999999996</v>
+        <v>0.57777777777777772</v>
       </c>
     </row>
   </sheetData>
@@ -3639,7 +3756,7 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3662,49 +3779,49 @@
         <v>187</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>224</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -3712,58 +3829,58 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>172</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="L2" s="12" t="s">
         <v>73</v>
       </c>
       <c r="M2" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="R2" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="N2" t="s">
+      <c r="S2" t="s">
         <v>250</v>
-      </c>
-      <c r="O2" t="s">
-        <v>251</v>
-      </c>
-      <c r="P2" t="s">
-        <v>252</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>253</v>
-      </c>
-      <c r="R2" t="s">
-        <v>254</v>
-      </c>
-      <c r="S2" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -3771,10 +3888,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -3783,46 +3900,46 @@
         <v>31</v>
       </c>
       <c r="F3" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="L3" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="M3" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="O3" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="P3" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="Q3" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="R3" s="12" t="s">
         <v>290</v>
       </c>
-      <c r="N3" t="s">
+      <c r="S3" t="s">
         <v>291</v>
-      </c>
-      <c r="O3" t="s">
-        <v>292</v>
-      </c>
-      <c r="P3" t="s">
-        <v>293</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>294</v>
-      </c>
-      <c r="R3" t="s">
-        <v>295</v>
-      </c>
-      <c r="S3" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -3830,10 +3947,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -3845,43 +3962,43 @@
         <v>51</v>
       </c>
       <c r="G4" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="L4" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="M4" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="N4" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="O4" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="P4" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q4" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="R4" s="12" t="s">
         <v>236</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="S4" t="s">
         <v>237</v>
-      </c>
-      <c r="N4" t="s">
-        <v>238</v>
-      </c>
-      <c r="O4" t="s">
-        <v>239</v>
-      </c>
-      <c r="P4" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>240</v>
-      </c>
-      <c r="R4" t="s">
-        <v>241</v>
-      </c>
-      <c r="S4" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -3889,58 +4006,58 @@
         <v>3</v>
       </c>
       <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
         <v>4</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="J5" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="K5" s="10" t="s">
         <v>269</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="L5" s="12" t="s">
         <v>270</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="M5" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="N5" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="O5" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="P5" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="Q5" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="R5" s="12" t="s">
         <v>276</v>
       </c>
-      <c r="N5" t="s">
+      <c r="S5" t="s">
         <v>277</v>
-      </c>
-      <c r="O5" t="s">
-        <v>278</v>
-      </c>
-      <c r="P5" t="s">
-        <v>279</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>280</v>
-      </c>
-      <c r="R5" t="s">
-        <v>281</v>
-      </c>
-      <c r="S5" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -3948,58 +4065,58 @@
         <v>4</v>
       </c>
       <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
         <v>5</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="J6" s="12" t="s">
         <v>297</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="K6" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="L6" s="12" t="s">
         <v>299</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>302</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>303</v>
-      </c>
-      <c r="L6" s="12" t="s">
-        <v>304</v>
       </c>
       <c r="M6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N6" t="s">
-        <v>305</v>
-      </c>
-      <c r="O6" t="s">
+      <c r="N6" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="O6" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="P6" t="s">
-        <v>306</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>307</v>
-      </c>
-      <c r="R6" t="s">
-        <v>308</v>
+      <c r="P6" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q6" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="R6" s="12" t="s">
+        <v>303</v>
       </c>
       <c r="S6" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -4007,58 +4124,58 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>105</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>23</v>
       </c>
       <c r="L7" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q7" s="12" t="s">
         <v>260</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="R7" s="12" t="s">
         <v>261</v>
       </c>
-      <c r="N7" t="s">
+      <c r="S7" t="s">
         <v>262</v>
-      </c>
-      <c r="O7" t="s">
-        <v>263</v>
-      </c>
-      <c r="P7" t="s">
-        <v>264</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>265</v>
-      </c>
-      <c r="R7" t="s">
-        <v>266</v>
-      </c>
-      <c r="S7" t="s">
-        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testing results updated for week 7
</commit_message>
<xml_diff>
--- a/AFootball testing results.xlsx
+++ b/AFootball testing results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Season results" sheetId="1" r:id="rId1"/>
@@ -1397,9 +1397,6 @@
     <t>AFNNET_logsig base rand</t>
   </si>
   <si>
-    <t>MIN(a) @ NYG(h) 2013 week 7</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -1983,6 +1980,33 @@
         <scheme val="minor"/>
       </rPr>
       <t>IND(h)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2013 week 7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MIN(a) @ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NYG(h)</t>
     </r>
     <r>
       <rPr>
@@ -2502,7 +2526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -2549,7 +2573,7 @@
       </c>
       <c r="C2">
         <f>'Week 4 results'!C2+'Week 5 results'!C2+'Week 6 results'!C2+'Week 7 results'!C2</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2">
         <f>'Week 4 results'!D2+'Week 5 results'!D2+'Week 6 results'!D2+'Week 7 results'!D2</f>
@@ -2557,15 +2581,15 @@
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E7" si="0">B2+C2+D2</f>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F2" s="14">
         <f t="shared" ref="F2:F7" si="1">B2/(E2-D2)</f>
-        <v>0.59090909090909094</v>
+        <v>0.57777777777777772</v>
       </c>
       <c r="G2" s="14">
         <f t="shared" ref="G2:G7" si="2">B2/E2</f>
-        <v>0.57777777777777772</v>
+        <v>0.56521739130434778</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2578,7 +2602,7 @@
       </c>
       <c r="C3">
         <f>'Week 4 results'!C3+'Week 5 results'!C3+'Week 6 results'!C3+'Week 7 results'!C3</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3">
         <f>'Week 4 results'!D3+'Week 5 results'!D3+'Week 6 results'!D3+'Week 7 results'!D3</f>
@@ -2586,15 +2610,15 @@
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F3" s="14">
         <f t="shared" si="1"/>
-        <v>0.6428571428571429</v>
+        <v>0.62790697674418605</v>
       </c>
       <c r="G3" s="14">
         <f t="shared" si="2"/>
-        <v>0.6</v>
+        <v>0.58695652173913049</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2607,7 +2631,7 @@
       </c>
       <c r="C4">
         <f>'Week 4 results'!C4+'Week 5 results'!C4+'Week 6 results'!C4+'Week 7 results'!C4</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4">
         <f>'Week 4 results'!D4+'Week 5 results'!D4+'Week 6 results'!D4+'Week 7 results'!D4</f>
@@ -2615,15 +2639,15 @@
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F4" s="14">
         <f t="shared" si="1"/>
-        <v>0.70454545454545459</v>
+        <v>0.68888888888888888</v>
       </c>
       <c r="G4" s="14">
         <f t="shared" si="2"/>
-        <v>0.68888888888888888</v>
+        <v>0.67391304347826086</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2636,7 +2660,7 @@
       </c>
       <c r="C5">
         <f>'Week 4 results'!C5+'Week 5 results'!C5+'Week 6 results'!C5+'Week 7 results'!C5</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5">
         <f>'Week 4 results'!D5+'Week 5 results'!D5+'Week 6 results'!D5+'Week 7 results'!D5</f>
@@ -2644,15 +2668,15 @@
       </c>
       <c r="E5">
         <f>B5+C5+D5</f>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F5" s="14">
         <f t="shared" si="1"/>
-        <v>0.69230769230769229</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="G5" s="14">
         <f t="shared" si="2"/>
-        <v>0.6</v>
+        <v>0.58695652173913049</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2665,7 +2689,7 @@
       </c>
       <c r="C6">
         <f>'Week 4 results'!C6+'Week 5 results'!C6+'Week 6 results'!C6+'Week 7 results'!C6</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6">
         <f>'Week 4 results'!D6+'Week 5 results'!D6+'Week 6 results'!D6+'Week 7 results'!D6</f>
@@ -2673,15 +2697,15 @@
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F6" s="14">
         <f t="shared" si="1"/>
-        <v>0.6097560975609756</v>
+        <v>0.59523809523809523</v>
       </c>
       <c r="G6" s="14">
         <f t="shared" si="2"/>
-        <v>0.55555555555555558</v>
+        <v>0.54347826086956519</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2694,7 +2718,7 @@
       </c>
       <c r="C7">
         <f>'Week 4 results'!C7+'Week 5 results'!C7+'Week 6 results'!C7+'Week 7 results'!C6</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D7">
         <f>'Week 4 results'!D7+'Week 5 results'!D7+'Week 6 results'!D7+'Week 7 results'!D7</f>
@@ -2702,15 +2726,15 @@
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F7" s="14">
         <f t="shared" si="1"/>
-        <v>0.59090909090909094</v>
+        <v>0.57777777777777772</v>
       </c>
       <c r="G7" s="14">
         <f t="shared" si="2"/>
-        <v>0.57777777777777772</v>
+        <v>0.56521739130434778</v>
       </c>
     </row>
   </sheetData>
@@ -3755,8 +3779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3779,49 +3803,49 @@
         <v>187</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>317</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -3832,55 +3856,55 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="12" t="s">
         <v>239</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>240</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>172</v>
       </c>
       <c r="I2" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="J2" s="12" t="s">
         <v>241</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="K2" s="7" t="s">
         <v>242</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>243</v>
       </c>
       <c r="L2" s="12" t="s">
         <v>73</v>
       </c>
       <c r="M2" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="N2" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="O2" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="P2" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="Q2" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="R2" s="12" t="s">
         <v>248</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="S2" s="12" t="s">
         <v>249</v>
-      </c>
-      <c r="S2" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -3891,7 +3915,7 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -3900,46 +3924,46 @@
         <v>31</v>
       </c>
       <c r="F3" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>278</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="H3" s="12" t="s">
         <v>279</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="I3" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="J3" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="K3" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="L3" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="M3" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="O3" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="P3" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="Q3" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="R3" s="12" t="s">
         <v>289</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="S3" s="12" t="s">
         <v>290</v>
-      </c>
-      <c r="S3" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -3950,7 +3974,7 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -3962,43 +3986,43 @@
         <v>51</v>
       </c>
       <c r="G4" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="H4" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="I4" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="J4" s="12" t="s">
         <v>228</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="K4" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="L4" s="12" t="s">
         <v>230</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="M4" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="N4" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="O4" s="7" t="s">
         <v>233</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>234</v>
       </c>
       <c r="P4" s="7" t="s">
         <v>172</v>
       </c>
       <c r="Q4" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="R4" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="R4" s="12" t="s">
+      <c r="S4" s="12" t="s">
         <v>236</v>
-      </c>
-      <c r="S4" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -4009,55 +4033,55 @@
         <v>8</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="G5" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="H5" s="12" t="s">
         <v>265</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="I5" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="J5" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="K5" s="10" t="s">
         <v>268</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="L5" s="12" t="s">
         <v>269</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="M5" s="7" t="s">
         <v>270</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="N5" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="O5" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="O5" s="7" t="s">
+      <c r="P5" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="P5" s="7" t="s">
+      <c r="Q5" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="Q5" s="7" t="s">
+      <c r="R5" s="12" t="s">
         <v>275</v>
       </c>
-      <c r="R5" s="12" t="s">
+      <c r="S5" s="12" t="s">
         <v>276</v>
-      </c>
-      <c r="S5" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -4068,55 +4092,55 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="G6" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="12" t="s">
         <v>294</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="I6" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="J6" s="12" t="s">
         <v>296</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="K6" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="L6" s="12" t="s">
         <v>298</v>
-      </c>
-      <c r="L6" s="12" t="s">
-        <v>299</v>
       </c>
       <c r="M6" s="7" t="s">
         <v>12</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="O6" s="7" t="s">
         <v>116</v>
       </c>
       <c r="P6" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="Q6" s="12" t="s">
         <v>301</v>
       </c>
-      <c r="Q6" s="12" t="s">
+      <c r="R6" s="12" t="s">
         <v>302</v>
       </c>
-      <c r="R6" s="12" t="s">
+      <c r="S6" s="12" t="s">
         <v>303</v>
-      </c>
-      <c r="S6" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -4127,55 +4151,55 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>251</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>252</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>105</v>
       </c>
       <c r="I7" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="J7" s="12" t="s">
         <v>253</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>254</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>23</v>
       </c>
       <c r="L7" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="M7" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="N7" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="N7" s="7" t="s">
+      <c r="O7" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="O7" s="7" t="s">
+      <c r="P7" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="P7" s="7" t="s">
+      <c r="Q7" s="12" t="s">
         <v>259</v>
       </c>
-      <c r="Q7" s="12" t="s">
+      <c r="R7" s="12" t="s">
         <v>260</v>
       </c>
-      <c r="R7" s="12" t="s">
+      <c r="S7" s="12" t="s">
         <v>261</v>
-      </c>
-      <c r="S7" t="s">
-        <v>262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final week 7 results
</commit_message>
<xml_diff>
--- a/AFootball testing results.xlsx
+++ b/AFootball testing results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Season results" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Week 5 results" sheetId="3" r:id="rId3"/>
     <sheet name="Week 6 results" sheetId="4" r:id="rId4"/>
     <sheet name="Week 7 results" sheetId="5" r:id="rId5"/>
+    <sheet name="Week 8 results" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="318">
   <si>
     <t>AF613_logsig base randomized w&amp;b*</t>
   </si>
@@ -2526,7 +2527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -3780,7 +3781,7 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B1" sqref="B1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4206,4 +4207,121 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="5" max="19" width="51.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
testing results spreadsheet updated for week 8
</commit_message>
<xml_diff>
--- a/AFootball testing results.xlsx
+++ b/AFootball testing results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="342">
   <si>
     <t>AF613_logsig base randomized w&amp;b*</t>
   </si>
@@ -2019,6 +2019,99 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> 2013 week 7</t>
+    </r>
+  </si>
+  <si>
+    <t>NYG(a) @ PHI(h) 2013 week 8</t>
+  </si>
+  <si>
+    <t>SF(a) @ JAC(h) 2013 week 8</t>
+  </si>
+  <si>
+    <t>DAL(a) @ DET(h) 2013 week 8</t>
+  </si>
+  <si>
+    <t>CLE(a) @ KC(h) 2013 week 8</t>
+  </si>
+  <si>
+    <t>MIA(a) @ NE(h) 2013 week 8</t>
+  </si>
+  <si>
+    <t>BUF(a) @ NO(h) 2013 week 8</t>
+  </si>
+  <si>
+    <t>PIT(a) @ OAK(h) 2013 week 8</t>
+  </si>
+  <si>
+    <t>NYJ(a) @ CIN(h) 2013 week 8</t>
+  </si>
+  <si>
+    <t>WAS(a) @ DEN(h) 2013 week 8</t>
+  </si>
+  <si>
+    <t>ATL(a) @ ARI(h) 2013 week 8</t>
+  </si>
+  <si>
+    <t>GB(a) @ MIN(h) 2013 week 8</t>
+  </si>
+  <si>
+    <t>SEA(a) @ STL(h) 2013 week 8</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.0004 / ON002(away win): 0.9995</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.7312 / ON002(away win): 0.2687</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.0215 / ON002(away win): 0.9784</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.3261 / ON002(away win): 0.6738</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9983 / ON002(away win): 0.0016</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.0125 / ON002(away win): 0.9874</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9615 / ON002(away win): 0.0384</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.7056 / ON002(away win): 0.2943</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.0016 / ON002(away win): 0.9983</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.000004 / ON002(away win): 0.9999</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.0000009 / ON002(away win): 0.9999</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CAR(a)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> @ TB(h) 2013 week 8</t>
     </r>
   </si>
 </sst>
@@ -2133,7 +2226,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2165,6 +2258,9 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2528,7 +2624,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2569,15 +2665,15 @@
         <v>223</v>
       </c>
       <c r="B2">
-        <f>'Week 4 results'!B2+'Week 5 results'!B2+'Week 6 results'!B2+'Week 7 results'!B2</f>
+        <f>'Week 4 results'!B2+'Week 5 results'!B2+'Week 6 results'!B2+'Week 7 results'!B2+'Week 8 results'!B2</f>
         <v>26</v>
       </c>
       <c r="C2">
-        <f>'Week 4 results'!C2+'Week 5 results'!C2+'Week 6 results'!C2+'Week 7 results'!C2</f>
+        <f>'Week 4 results'!C2+'Week 5 results'!C2+'Week 6 results'!C2+'Week 7 results'!C2+'Week 8 results'!C2</f>
         <v>19</v>
       </c>
       <c r="D2">
-        <f>'Week 4 results'!D2+'Week 5 results'!D2+'Week 6 results'!D2+'Week 7 results'!D2</f>
+        <f>'Week 4 results'!D2+'Week 5 results'!D2+'Week 6 results'!D2+'Week 7 results'!D2+'Week 8 results'!D2</f>
         <v>1</v>
       </c>
       <c r="E2">
@@ -2598,15 +2694,15 @@
         <v>222</v>
       </c>
       <c r="B3">
-        <f>'Week 4 results'!B3+'Week 5 results'!B3+'Week 6 results'!B3+'Week 7 results'!B3</f>
+        <f>'Week 4 results'!B3+'Week 5 results'!B3+'Week 6 results'!B3+'Week 7 results'!B3+'Week 8 results'!B3</f>
         <v>27</v>
       </c>
       <c r="C3">
-        <f>'Week 4 results'!C3+'Week 5 results'!C3+'Week 6 results'!C3+'Week 7 results'!C3</f>
+        <f>'Week 4 results'!C3+'Week 5 results'!C3+'Week 6 results'!C3+'Week 7 results'!C3+'Week 8 results'!C3</f>
         <v>16</v>
       </c>
       <c r="D3">
-        <f>'Week 4 results'!D3+'Week 5 results'!D3+'Week 6 results'!D3+'Week 7 results'!D3</f>
+        <f>'Week 4 results'!D3+'Week 5 results'!D3+'Week 6 results'!D3+'Week 7 results'!D3+'Week 8 results'!D3</f>
         <v>3</v>
       </c>
       <c r="E3">
@@ -2627,28 +2723,28 @@
         <v>221</v>
       </c>
       <c r="B4">
-        <f>'Week 4 results'!B4+'Week 5 results'!B4+'Week 6 results'!B4+'Week 7 results'!B4</f>
-        <v>31</v>
+        <f>'Week 4 results'!B4+'Week 5 results'!B4+'Week 6 results'!B4+'Week 7 results'!B4+'Week 8 results'!B4</f>
+        <v>32</v>
       </c>
       <c r="C4">
-        <f>'Week 4 results'!C4+'Week 5 results'!C4+'Week 6 results'!C4+'Week 7 results'!C4</f>
+        <f>'Week 4 results'!C4+'Week 5 results'!C4+'Week 6 results'!C4+'Week 7 results'!C4+'Week 8 results'!C4</f>
         <v>14</v>
       </c>
       <c r="D4">
-        <f>'Week 4 results'!D4+'Week 5 results'!D4+'Week 6 results'!D4+'Week 7 results'!D4</f>
+        <f>'Week 4 results'!D4+'Week 5 results'!D4+'Week 6 results'!D4+'Week 7 results'!D4+'Week 8 results'!D4</f>
         <v>1</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F4" s="14">
         <f t="shared" si="1"/>
-        <v>0.68888888888888888</v>
+        <v>0.69565217391304346</v>
       </c>
       <c r="G4" s="14">
         <f t="shared" si="2"/>
-        <v>0.67391304347826086</v>
+        <v>0.68085106382978722</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2656,15 +2752,15 @@
         <v>220</v>
       </c>
       <c r="B5">
-        <f>'Week 4 results'!B5+'Week 5 results'!B5+'Week 6 results'!B5+'Week 7 results'!B5</f>
+        <f>'Week 4 results'!B5+'Week 5 results'!B5+'Week 6 results'!B5+'Week 7 results'!B5+'Week 8 results'!B5</f>
         <v>27</v>
       </c>
       <c r="C5">
-        <f>'Week 4 results'!C5+'Week 5 results'!C5+'Week 6 results'!C5+'Week 7 results'!C5</f>
+        <f>'Week 4 results'!C5+'Week 5 results'!C5+'Week 6 results'!C5+'Week 7 results'!C5+'Week 8 results'!C5</f>
         <v>13</v>
       </c>
       <c r="D5">
-        <f>'Week 4 results'!D5+'Week 5 results'!D5+'Week 6 results'!D5+'Week 7 results'!D5</f>
+        <f>'Week 4 results'!D5+'Week 5 results'!D5+'Week 6 results'!D5+'Week 7 results'!D5+'Week 8 results'!D5</f>
         <v>6</v>
       </c>
       <c r="E5">
@@ -2685,15 +2781,15 @@
         <v>219</v>
       </c>
       <c r="B6">
-        <f>'Week 4 results'!B6+'Week 5 results'!B6+'Week 6 results'!B6+'Week 7 results'!B6</f>
+        <f>'Week 4 results'!B6+'Week 5 results'!B6+'Week 6 results'!B6+'Week 7 results'!B6+'Week 8 results'!B6</f>
         <v>25</v>
       </c>
       <c r="C6">
-        <f>'Week 4 results'!C6+'Week 5 results'!C6+'Week 6 results'!C6+'Week 7 results'!C6</f>
+        <f>'Week 4 results'!C6+'Week 5 results'!C6+'Week 6 results'!C6+'Week 7 results'!C6+'Week 8 results'!C6</f>
         <v>17</v>
       </c>
       <c r="D6">
-        <f>'Week 4 results'!D6+'Week 5 results'!D6+'Week 6 results'!D6+'Week 7 results'!D6</f>
+        <f>'Week 4 results'!D6+'Week 5 results'!D6+'Week 6 results'!D6+'Week 7 results'!D6+'Week 8 results'!D6</f>
         <v>4</v>
       </c>
       <c r="E6">
@@ -2714,15 +2810,15 @@
         <v>218</v>
       </c>
       <c r="B7">
-        <f>'Week 4 results'!B7+'Week 5 results'!B7+'Week 6 results'!B7+'Week 7 results'!B7</f>
+        <f>'Week 4 results'!B7+'Week 5 results'!B7+'Week 6 results'!B7+'Week 7 results'!B7+'Week 8 results'!B7</f>
         <v>26</v>
       </c>
       <c r="C7">
-        <f>'Week 4 results'!C7+'Week 5 results'!C7+'Week 6 results'!C7+'Week 7 results'!C6</f>
+        <f>'Week 4 results'!C7+'Week 5 results'!C7+'Week 6 results'!C7+'Week 7 results'!C7+'Week 8 results'!C7</f>
         <v>19</v>
       </c>
       <c r="D7">
-        <f>'Week 4 results'!D7+'Week 5 results'!D7+'Week 6 results'!D7+'Week 7 results'!D7</f>
+        <f>'Week 4 results'!D7+'Week 5 results'!D7+'Week 6 results'!D7+'Week 7 results'!D7+'Week 8 results'!D7</f>
         <v>1</v>
       </c>
       <c r="E7">
@@ -3781,7 +3877,7 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1048576"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4211,7 +4307,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
@@ -4220,24 +4316,66 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
-    <col min="5" max="19" width="51.7109375" customWidth="1"/>
+    <col min="5" max="17" width="51.7109375" customWidth="1"/>
+    <col min="18" max="18" width="12" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:18">
+      <c r="A1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="16" t="s">
         <v>187</v>
       </c>
+      <c r="E1" s="16" t="s">
+        <v>341</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>319</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>320</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>321</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>322</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>323</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>324</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>325</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>326</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>327</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>328</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>329</v>
+      </c>
+      <c r="R1" s="16"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:18">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -4251,7 +4389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:18">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -4265,12 +4403,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:18">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -4278,8 +4416,47 @@
       <c r="D4">
         <v>0</v>
       </c>
+      <c r="E4" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="F4" t="s">
+        <v>331</v>
+      </c>
+      <c r="G4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4" t="s">
+        <v>332</v>
+      </c>
+      <c r="I4" t="s">
+        <v>231</v>
+      </c>
+      <c r="J4" t="s">
+        <v>333</v>
+      </c>
+      <c r="K4" t="s">
+        <v>334</v>
+      </c>
+      <c r="L4" t="s">
+        <v>335</v>
+      </c>
+      <c r="M4" t="s">
+        <v>336</v>
+      </c>
+      <c r="N4" t="s">
+        <v>337</v>
+      </c>
+      <c r="O4" t="s">
+        <v>338</v>
+      </c>
+      <c r="P4" t="s">
+        <v>339</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>340</v>
+      </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:18">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -4293,7 +4470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:18">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -4307,7 +4484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:18">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -4323,5 +4500,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Week 8 testing spreadsheet update
</commit_message>
<xml_diff>
--- a/AFootball testing results.xlsx
+++ b/AFootball testing results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Season results" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="402">
   <si>
     <t>AF613_logsig base randomized w&amp;b*</t>
   </si>
@@ -2113,6 +2113,186 @@
       </rPr>
       <t xml:space="preserve"> @ TB(h) 2013 week 8</t>
     </r>
+  </si>
+  <si>
+    <t>ON001(home win): 0.0003 / ON002(away win): 0.9996</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9905  / ON002(away win): 0.0094</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.0023  / ON002(away win): 0.9976</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.1874  / ON002(away win): 0.8125</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9901  / ON002(away win): 0.0098</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9390  / ON002(away win): 0.0609</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9996  / ON002(away win): 0.0003</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.1096  / ON002(away win): 0.8903</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9918  / ON002(away win): 0.0081</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9986  / ON002(away win): 0.0013</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.2467  / ON002(away win): 0.7532</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.0001  / ON002(away win): 0.9998</t>
+  </si>
+  <si>
+    <t>ON001(home win): 1.9e-9  / ON002(away win): 0.9999</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9999  / ON002(away win): 0.00003</t>
+  </si>
+  <si>
+    <t>ON001(home win): 4.1e-9  / ON002(away win): 0.9999</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.0225  / ON002(away win): 0.9771</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9987  / ON002(away win): 0.0012</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0. 0727 / ON002(away win): 0.9234</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9999  / ON002(away win): 1.08e-8</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.8273  / ON002(away win): 0.1689</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9994  / ON002(away win): 0.0004</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9999  / ON002(away win): 2.0e-8</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.0012  / ON002(away win): 0.9987</t>
+  </si>
+  <si>
+    <t>ON001(home win): 2.3e-8  / ON002(away win): 0.9999</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9999  / ON002(away win): 0.0000003</t>
+  </si>
+  <si>
+    <t>ON001(home win): 1.8e-11  / ON002(away win): 0.9999</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.4729  / ON002(away win): 0.5269</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9905  / ON002(away win): 0.0091</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.6946  / ON002(away win): 0.3089</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.0063  / ON002(away win): 0.9939</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.6489  / ON002(away win): 0.3507</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9998  / ON002(away win): 0.0001</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.0010  / ON002(away win): 0.9990</t>
+  </si>
+  <si>
+    <t>ON001(home win): 1.1e-9  / ON002(away win): 0.9999</t>
+  </si>
+  <si>
+    <t>ON001(home win): 1.2e-11  / ON002(away win): 0.9999</t>
+  </si>
+  <si>
+    <t>ON001(home win): 3.8e-9  / ON002(away win): 0.9999</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9997  / ON002(away win): 0.0002</t>
+  </si>
+  <si>
+    <t>ON001(home win): 1.7e-8  / ON002(away win): 0.9999</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.2743  / ON002(away win): 0.7331</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9999  / ON002(away win): 0.00002</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9162  / ON002(away win): 0.0832</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9999  / ON002(away win): 0.000002</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9932  / ON002(away win): 0.0068</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9945  / ON002(away win): 0.0052</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.00002  / ON002(away win): 0.9999</t>
+  </si>
+  <si>
+    <t>ON001(home win): 9.9e-7  / ON002(away win): 0.9999</t>
+  </si>
+  <si>
+    <t>ON001(home win): 6.1e-7  / ON002(away win): 0.9999</t>
+  </si>
+  <si>
+    <t>ON001(home win): 6.7e-14  / ON002(away win): 0.9999</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9999  / ON002(away win): 3.6e-10</t>
+  </si>
+  <si>
+    <t>ON001(home win): 7.3e-14  / ON002(away win): 0.999</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.000002  / ON002(away win): 0.9999</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9999  / ON002(away win):1.1e-11</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.1677  / ON002(away win): 0.8322</t>
+  </si>
+  <si>
+    <t>ON001(home win): 1.0  / ON002(away win): 5.5e-18</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9999  / ON002(away win): 1.9e-9</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9999  / ON002(away win): 1.9e-11</t>
+  </si>
+  <si>
+    <t>ON001(home win): 1.0  / ON002(away win): 1.2e-25</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.0350  / ON002(away win): 0.9649</t>
+  </si>
+  <si>
+    <t>ON001(home win): 6.8e-14  / ON002(away win): 0.9999</t>
+  </si>
+  <si>
+    <t>ON001(home win): 1.5e-13  / ON002(away win): 0.9999</t>
   </si>
 </sst>
 </file>
@@ -2623,8 +2803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2666,7 +2846,7 @@
       </c>
       <c r="B2">
         <f>'Week 4 results'!B2+'Week 5 results'!B2+'Week 6 results'!B2+'Week 7 results'!B2+'Week 8 results'!B2</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C2">
         <f>'Week 4 results'!C2+'Week 5 results'!C2+'Week 6 results'!C2+'Week 7 results'!C2+'Week 8 results'!C2</f>
@@ -2678,15 +2858,15 @@
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E7" si="0">B2+C2+D2</f>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F2" s="14">
         <f t="shared" ref="F2:F7" si="1">B2/(E2-D2)</f>
-        <v>0.57777777777777772</v>
+        <v>0.58695652173913049</v>
       </c>
       <c r="G2" s="14">
         <f t="shared" ref="G2:G7" si="2">B2/E2</f>
-        <v>0.56521739130434778</v>
+        <v>0.57446808510638303</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2695,7 +2875,7 @@
       </c>
       <c r="B3">
         <f>'Week 4 results'!B3+'Week 5 results'!B3+'Week 6 results'!B3+'Week 7 results'!B3+'Week 8 results'!B3</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3">
         <f>'Week 4 results'!C3+'Week 5 results'!C3+'Week 6 results'!C3+'Week 7 results'!C3+'Week 8 results'!C3</f>
@@ -2707,15 +2887,15 @@
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F3" s="14">
         <f t="shared" si="1"/>
-        <v>0.62790697674418605</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="G3" s="14">
         <f t="shared" si="2"/>
-        <v>0.58695652173913049</v>
+        <v>0.5957446808510638</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2753,7 +2933,7 @@
       </c>
       <c r="B5">
         <f>'Week 4 results'!B5+'Week 5 results'!B5+'Week 6 results'!B5+'Week 7 results'!B5+'Week 8 results'!B5</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C5">
         <f>'Week 4 results'!C5+'Week 5 results'!C5+'Week 6 results'!C5+'Week 7 results'!C5+'Week 8 results'!C5</f>
@@ -2761,19 +2941,19 @@
       </c>
       <c r="D5">
         <f>'Week 4 results'!D5+'Week 5 results'!D5+'Week 6 results'!D5+'Week 7 results'!D5+'Week 8 results'!D5</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E5">
         <f>B5+C5+D5</f>
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F5" s="14">
         <f t="shared" si="1"/>
-        <v>0.67500000000000004</v>
+        <v>0.68292682926829273</v>
       </c>
       <c r="G5" s="14">
         <f t="shared" si="2"/>
-        <v>0.58695652173913049</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2782,7 +2962,7 @@
       </c>
       <c r="B6">
         <f>'Week 4 results'!B6+'Week 5 results'!B6+'Week 6 results'!B6+'Week 7 results'!B6+'Week 8 results'!B6</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6">
         <f>'Week 4 results'!C6+'Week 5 results'!C6+'Week 6 results'!C6+'Week 7 results'!C6+'Week 8 results'!C6</f>
@@ -2794,15 +2974,15 @@
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F6" s="14">
         <f t="shared" si="1"/>
-        <v>0.59523809523809523</v>
+        <v>0.60465116279069764</v>
       </c>
       <c r="G6" s="14">
         <f t="shared" si="2"/>
-        <v>0.54347826086956519</v>
+        <v>0.55319148936170215</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2811,7 +2991,7 @@
       </c>
       <c r="B7">
         <f>'Week 4 results'!B7+'Week 5 results'!B7+'Week 6 results'!B7+'Week 7 results'!B7+'Week 8 results'!B7</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7">
         <f>'Week 4 results'!C7+'Week 5 results'!C7+'Week 6 results'!C7+'Week 7 results'!C7+'Week 8 results'!C7</f>
@@ -2823,15 +3003,15 @@
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F7" s="14">
         <f t="shared" si="1"/>
-        <v>0.57777777777777772</v>
+        <v>0.58695652173913049</v>
       </c>
       <c r="G7" s="14">
         <f t="shared" si="2"/>
-        <v>0.56521739130434778</v>
+        <v>0.57446808510638303</v>
       </c>
     </row>
   </sheetData>
@@ -4309,8 +4489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4380,13 +4560,52 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="F2" t="s">
+        <v>355</v>
+      </c>
+      <c r="G2" t="s">
+        <v>356</v>
+      </c>
+      <c r="H2" t="s">
+        <v>357</v>
+      </c>
+      <c r="I2" t="s">
+        <v>358</v>
+      </c>
+      <c r="J2" t="s">
+        <v>359</v>
+      </c>
+      <c r="K2" t="s">
+        <v>360</v>
+      </c>
+      <c r="L2" t="s">
+        <v>361</v>
+      </c>
+      <c r="M2" t="s">
+        <v>362</v>
+      </c>
+      <c r="N2" t="s">
+        <v>363</v>
+      </c>
+      <c r="O2" t="s">
+        <v>275</v>
+      </c>
+      <c r="P2" t="s">
+        <v>353</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -4394,13 +4613,52 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="F3" t="s">
+        <v>343</v>
+      </c>
+      <c r="G3" t="s">
+        <v>344</v>
+      </c>
+      <c r="H3" t="s">
+        <v>345</v>
+      </c>
+      <c r="I3" t="s">
+        <v>346</v>
+      </c>
+      <c r="J3" t="s">
+        <v>347</v>
+      </c>
+      <c r="K3" t="s">
+        <v>348</v>
+      </c>
+      <c r="L3" t="s">
+        <v>349</v>
+      </c>
+      <c r="M3" t="s">
+        <v>350</v>
+      </c>
+      <c r="N3" t="s">
+        <v>351</v>
+      </c>
+      <c r="O3" t="s">
+        <v>352</v>
+      </c>
+      <c r="P3" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -4457,17 +4715,56 @@
       </c>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="3" t="s">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="F5" t="s">
+        <v>366</v>
+      </c>
+      <c r="G5" t="s">
+        <v>367</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="I5" t="s">
+        <v>369</v>
+      </c>
+      <c r="J5" t="s">
+        <v>370</v>
+      </c>
+      <c r="K5" t="s">
+        <v>265</v>
+      </c>
+      <c r="L5" t="s">
+        <v>371</v>
+      </c>
+      <c r="M5" t="s">
+        <v>372</v>
+      </c>
+      <c r="N5" t="s">
+        <v>373</v>
+      </c>
+      <c r="O5" t="s">
+        <v>374</v>
+      </c>
+      <c r="P5" t="s">
+        <v>375</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -4475,7 +4772,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -4483,19 +4780,97 @@
       <c r="D6">
         <v>0</v>
       </c>
+      <c r="E6" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="F6" t="s">
+        <v>378</v>
+      </c>
+      <c r="G6" t="s">
+        <v>379</v>
+      </c>
+      <c r="H6" t="s">
+        <v>380</v>
+      </c>
+      <c r="I6" t="s">
+        <v>381</v>
+      </c>
+      <c r="J6" t="s">
+        <v>382</v>
+      </c>
+      <c r="K6" t="s">
+        <v>383</v>
+      </c>
+      <c r="L6" t="s">
+        <v>353</v>
+      </c>
+      <c r="M6" t="s">
+        <v>384</v>
+      </c>
+      <c r="N6" t="s">
+        <v>385</v>
+      </c>
+      <c r="O6" t="s">
+        <v>386</v>
+      </c>
+      <c r="P6" t="s">
+        <v>387</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="3" t="s">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
         <v>0</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="F7" t="s">
+        <v>390</v>
+      </c>
+      <c r="G7" t="s">
+        <v>391</v>
+      </c>
+      <c r="H7" t="s">
+        <v>392</v>
+      </c>
+      <c r="I7" t="s">
+        <v>393</v>
+      </c>
+      <c r="J7" t="s">
+        <v>394</v>
+      </c>
+      <c r="K7" t="s">
+        <v>395</v>
+      </c>
+      <c r="L7" t="s">
+        <v>396</v>
+      </c>
+      <c r="M7" t="s">
+        <v>397</v>
+      </c>
+      <c r="N7" t="s">
+        <v>398</v>
+      </c>
+      <c r="O7" t="s">
+        <v>399</v>
+      </c>
+      <c r="P7" t="s">
+        <v>400</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testing results spreadsheet for week 8 games
</commit_message>
<xml_diff>
--- a/AFootball testing results.xlsx
+++ b/AFootball testing results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Season results" sheetId="1" r:id="rId1"/>
@@ -2022,36 +2022,6 @@
     </r>
   </si>
   <si>
-    <t>NYG(a) @ PHI(h) 2013 week 8</t>
-  </si>
-  <si>
-    <t>SF(a) @ JAC(h) 2013 week 8</t>
-  </si>
-  <si>
-    <t>DAL(a) @ DET(h) 2013 week 8</t>
-  </si>
-  <si>
-    <t>CLE(a) @ KC(h) 2013 week 8</t>
-  </si>
-  <si>
-    <t>MIA(a) @ NE(h) 2013 week 8</t>
-  </si>
-  <si>
-    <t>BUF(a) @ NO(h) 2013 week 8</t>
-  </si>
-  <si>
-    <t>PIT(a) @ OAK(h) 2013 week 8</t>
-  </si>
-  <si>
-    <t>NYJ(a) @ CIN(h) 2013 week 8</t>
-  </si>
-  <si>
-    <t>WAS(a) @ DEN(h) 2013 week 8</t>
-  </si>
-  <si>
-    <t>ATL(a) @ ARI(h) 2013 week 8</t>
-  </si>
-  <si>
     <t>GB(a) @ MIN(h) 2013 week 8</t>
   </si>
   <si>
@@ -2293,6 +2263,270 @@
   </si>
   <si>
     <t>ON001(home win): 1.5e-13  / ON002(away win): 0.9999</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NYG(a)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> @ PHI(h) 2013 week 8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SF(a)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> @ JAC(h) 2013 week 8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">DAL(a) @ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DET(h)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2013 week 8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CLE(a) @ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KC(h)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2013 week 8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MIA(a) @ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NE(h)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2013 week 8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">BUF(a) @ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NO(h)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2013 week 8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PIT(a) @ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OAK(h)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2013 week 8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">NYJ(a) @ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CIN(h)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2013 week 8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">WAS(a) @ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DEN(h)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2013 week 8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ATL(a) @ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ARI(h)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2013 week 8</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2803,7 +3037,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -2846,11 +3080,11 @@
       </c>
       <c r="B2">
         <f>'Week 4 results'!B2+'Week 5 results'!B2+'Week 6 results'!B2+'Week 7 results'!B2+'Week 8 results'!B2</f>
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C2">
         <f>'Week 4 results'!C2+'Week 5 results'!C2+'Week 6 results'!C2+'Week 7 results'!C2+'Week 8 results'!C2</f>
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D2">
         <f>'Week 4 results'!D2+'Week 5 results'!D2+'Week 6 results'!D2+'Week 7 results'!D2+'Week 8 results'!D2</f>
@@ -2858,15 +3092,15 @@
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E7" si="0">B2+C2+D2</f>
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="F2" s="14">
         <f t="shared" ref="F2:F7" si="1">B2/(E2-D2)</f>
-        <v>0.58695652173913049</v>
+        <v>0.5892857142857143</v>
       </c>
       <c r="G2" s="14">
         <f t="shared" ref="G2:G7" si="2">B2/E2</f>
-        <v>0.57446808510638303</v>
+        <v>0.57894736842105265</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2875,11 +3109,11 @@
       </c>
       <c r="B3">
         <f>'Week 4 results'!B3+'Week 5 results'!B3+'Week 6 results'!B3+'Week 7 results'!B3+'Week 8 results'!B3</f>
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C3">
         <f>'Week 4 results'!C3+'Week 5 results'!C3+'Week 6 results'!C3+'Week 7 results'!C3+'Week 8 results'!C3</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D3">
         <f>'Week 4 results'!D3+'Week 5 results'!D3+'Week 6 results'!D3+'Week 7 results'!D3+'Week 8 results'!D3</f>
@@ -2887,15 +3121,15 @@
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="F3" s="14">
         <f t="shared" si="1"/>
-        <v>0.63636363636363635</v>
+        <v>0.62962962962962965</v>
       </c>
       <c r="G3" s="14">
         <f t="shared" si="2"/>
-        <v>0.5957446808510638</v>
+        <v>0.59649122807017541</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2904,11 +3138,11 @@
       </c>
       <c r="B4">
         <f>'Week 4 results'!B4+'Week 5 results'!B4+'Week 6 results'!B4+'Week 7 results'!B4+'Week 8 results'!B4</f>
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C4">
         <f>'Week 4 results'!C4+'Week 5 results'!C4+'Week 6 results'!C4+'Week 7 results'!C4+'Week 8 results'!C4</f>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D4">
         <f>'Week 4 results'!D4+'Week 5 results'!D4+'Week 6 results'!D4+'Week 7 results'!D4+'Week 8 results'!D4</f>
@@ -2916,15 +3150,15 @@
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="F4" s="14">
         <f t="shared" si="1"/>
-        <v>0.69565217391304346</v>
+        <v>0.6607142857142857</v>
       </c>
       <c r="G4" s="14">
         <f t="shared" si="2"/>
-        <v>0.68085106382978722</v>
+        <v>0.64912280701754388</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2933,11 +3167,11 @@
       </c>
       <c r="B5">
         <f>'Week 4 results'!B5+'Week 5 results'!B5+'Week 6 results'!B5+'Week 7 results'!B5+'Week 8 results'!B5</f>
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C5">
         <f>'Week 4 results'!C5+'Week 5 results'!C5+'Week 6 results'!C5+'Week 7 results'!C5+'Week 8 results'!C5</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D5">
         <f>'Week 4 results'!D5+'Week 5 results'!D5+'Week 6 results'!D5+'Week 7 results'!D5+'Week 8 results'!D5</f>
@@ -2945,15 +3179,15 @@
       </c>
       <c r="E5">
         <f>B5+C5+D5</f>
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="F5" s="14">
         <f t="shared" si="1"/>
-        <v>0.68292682926829273</v>
+        <v>0.68</v>
       </c>
       <c r="G5" s="14">
         <f t="shared" si="2"/>
-        <v>0.58333333333333337</v>
+        <v>0.59649122807017541</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2962,11 +3196,11 @@
       </c>
       <c r="B6">
         <f>'Week 4 results'!B6+'Week 5 results'!B6+'Week 6 results'!B6+'Week 7 results'!B6+'Week 8 results'!B6</f>
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C6">
         <f>'Week 4 results'!C6+'Week 5 results'!C6+'Week 6 results'!C6+'Week 7 results'!C6+'Week 8 results'!C6</f>
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D6">
         <f>'Week 4 results'!D6+'Week 5 results'!D6+'Week 6 results'!D6+'Week 7 results'!D6+'Week 8 results'!D6</f>
@@ -2974,15 +3208,15 @@
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="F6" s="14">
         <f t="shared" si="1"/>
-        <v>0.60465116279069764</v>
+        <v>0.60377358490566035</v>
       </c>
       <c r="G6" s="14">
         <f t="shared" si="2"/>
-        <v>0.55319148936170215</v>
+        <v>0.56140350877192979</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2991,11 +3225,11 @@
       </c>
       <c r="B7">
         <f>'Week 4 results'!B7+'Week 5 results'!B7+'Week 6 results'!B7+'Week 7 results'!B7+'Week 8 results'!B7</f>
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C7">
         <f>'Week 4 results'!C7+'Week 5 results'!C7+'Week 6 results'!C7+'Week 7 results'!C7+'Week 8 results'!C7</f>
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D7">
         <f>'Week 4 results'!D7+'Week 5 results'!D7+'Week 6 results'!D7+'Week 7 results'!D7+'Week 8 results'!D7</f>
@@ -3003,15 +3237,15 @@
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="F7" s="14">
         <f t="shared" si="1"/>
-        <v>0.58695652173913049</v>
+        <v>0.5892857142857143</v>
       </c>
       <c r="G7" s="14">
         <f t="shared" si="2"/>
-        <v>0.57446808510638303</v>
+        <v>0.57894736842105265</v>
       </c>
     </row>
   </sheetData>
@@ -4489,8 +4723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4515,43 +4749,43 @@
         <v>187</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="F1" s="16" t="s">
+        <v>392</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>393</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>394</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>395</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>397</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>398</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>399</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>400</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>401</v>
+      </c>
+      <c r="P1" s="16" t="s">
         <v>318</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="Q1" s="16" t="s">
         <v>319</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>320</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>321</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>322</v>
-      </c>
-      <c r="K1" s="16" t="s">
-        <v>323</v>
-      </c>
-      <c r="L1" s="16" t="s">
-        <v>324</v>
-      </c>
-      <c r="M1" s="16" t="s">
-        <v>325</v>
-      </c>
-      <c r="N1" s="16" t="s">
-        <v>326</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>327</v>
-      </c>
-      <c r="P1" s="16" t="s">
-        <v>328</v>
-      </c>
-      <c r="Q1" s="16" t="s">
-        <v>329</v>
       </c>
       <c r="R1" s="16"/>
     </row>
@@ -4560,52 +4794,52 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="P2" t="s">
+        <v>343</v>
+      </c>
+      <c r="Q2" t="s">
         <v>354</v>
-      </c>
-      <c r="F2" t="s">
-        <v>355</v>
-      </c>
-      <c r="G2" t="s">
-        <v>356</v>
-      </c>
-      <c r="H2" t="s">
-        <v>357</v>
-      </c>
-      <c r="I2" t="s">
-        <v>358</v>
-      </c>
-      <c r="J2" t="s">
-        <v>359</v>
-      </c>
-      <c r="K2" t="s">
-        <v>360</v>
-      </c>
-      <c r="L2" t="s">
-        <v>361</v>
-      </c>
-      <c r="M2" t="s">
-        <v>362</v>
-      </c>
-      <c r="N2" t="s">
-        <v>363</v>
-      </c>
-      <c r="O2" t="s">
-        <v>275</v>
-      </c>
-      <c r="P2" t="s">
-        <v>353</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -4613,52 +4847,52 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="O3" s="12" t="s">
         <v>342</v>
-      </c>
-      <c r="F3" t="s">
-        <v>343</v>
-      </c>
-      <c r="G3" t="s">
-        <v>344</v>
-      </c>
-      <c r="H3" t="s">
-        <v>345</v>
-      </c>
-      <c r="I3" t="s">
-        <v>346</v>
-      </c>
-      <c r="J3" t="s">
-        <v>347</v>
-      </c>
-      <c r="K3" t="s">
-        <v>348</v>
-      </c>
-      <c r="L3" t="s">
-        <v>349</v>
-      </c>
-      <c r="M3" t="s">
-        <v>350</v>
-      </c>
-      <c r="N3" t="s">
-        <v>351</v>
-      </c>
-      <c r="O3" t="s">
-        <v>352</v>
       </c>
       <c r="P3" t="s">
         <v>275</v>
       </c>
       <c r="Q3" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -4666,52 +4900,52 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="P4" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q4" t="s">
         <v>330</v>
-      </c>
-      <c r="F4" t="s">
-        <v>331</v>
-      </c>
-      <c r="G4" t="s">
-        <v>72</v>
-      </c>
-      <c r="H4" t="s">
-        <v>332</v>
-      </c>
-      <c r="I4" t="s">
-        <v>231</v>
-      </c>
-      <c r="J4" t="s">
-        <v>333</v>
-      </c>
-      <c r="K4" t="s">
-        <v>334</v>
-      </c>
-      <c r="L4" t="s">
-        <v>335</v>
-      </c>
-      <c r="M4" t="s">
-        <v>336</v>
-      </c>
-      <c r="N4" t="s">
-        <v>337</v>
-      </c>
-      <c r="O4" t="s">
-        <v>338</v>
-      </c>
-      <c r="P4" t="s">
-        <v>339</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -4719,52 +4953,52 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>356</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>361</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>364</v>
+      </c>
+      <c r="P5" t="s">
         <v>365</v>
       </c>
-      <c r="F5" t="s">
+      <c r="Q5" t="s">
         <v>366</v>
-      </c>
-      <c r="G5" t="s">
-        <v>367</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>368</v>
-      </c>
-      <c r="I5" t="s">
-        <v>369</v>
-      </c>
-      <c r="J5" t="s">
-        <v>370</v>
-      </c>
-      <c r="K5" t="s">
-        <v>265</v>
-      </c>
-      <c r="L5" t="s">
-        <v>371</v>
-      </c>
-      <c r="M5" t="s">
-        <v>372</v>
-      </c>
-      <c r="N5" t="s">
-        <v>373</v>
-      </c>
-      <c r="O5" t="s">
-        <v>374</v>
-      </c>
-      <c r="P5" t="s">
-        <v>375</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -4772,52 +5006,52 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>368</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>370</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>376</v>
+      </c>
+      <c r="P6" t="s">
         <v>377</v>
       </c>
-      <c r="F6" t="s">
+      <c r="Q6" t="s">
         <v>378</v>
-      </c>
-      <c r="G6" t="s">
-        <v>379</v>
-      </c>
-      <c r="H6" t="s">
-        <v>380</v>
-      </c>
-      <c r="I6" t="s">
-        <v>381</v>
-      </c>
-      <c r="J6" t="s">
-        <v>382</v>
-      </c>
-      <c r="K6" t="s">
-        <v>383</v>
-      </c>
-      <c r="L6" t="s">
-        <v>353</v>
-      </c>
-      <c r="M6" t="s">
-        <v>384</v>
-      </c>
-      <c r="N6" t="s">
-        <v>385</v>
-      </c>
-      <c r="O6" t="s">
-        <v>386</v>
-      </c>
-      <c r="P6" t="s">
-        <v>387</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -4825,52 +5059,52 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>380</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>382</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="O7" s="12" t="s">
         <v>389</v>
       </c>
-      <c r="F7" t="s">
+      <c r="P7" t="s">
         <v>390</v>
       </c>
-      <c r="G7" t="s">
+      <c r="Q7" t="s">
         <v>391</v>
-      </c>
-      <c r="H7" t="s">
-        <v>392</v>
-      </c>
-      <c r="I7" t="s">
-        <v>393</v>
-      </c>
-      <c r="J7" t="s">
-        <v>394</v>
-      </c>
-      <c r="K7" t="s">
-        <v>395</v>
-      </c>
-      <c r="L7" t="s">
-        <v>396</v>
-      </c>
-      <c r="M7" t="s">
-        <v>397</v>
-      </c>
-      <c r="N7" t="s">
-        <v>398</v>
-      </c>
-      <c r="O7" t="s">
-        <v>399</v>
-      </c>
-      <c r="P7" t="s">
-        <v>400</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testing results spreadsheet and week 9 data set
</commit_message>
<xml_diff>
--- a/AFootball testing results.xlsx
+++ b/AFootball testing results.xlsx
@@ -2022,9 +2022,6 @@
     </r>
   </si>
   <si>
-    <t>SEA(a) @ STL(h) 2013 week 8</t>
-  </si>
-  <si>
     <t>ON001(home win): 0.0004 / ON002(away win): 0.9995</t>
   </si>
   <si>
@@ -2547,6 +2544,30 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> @ MIN(h) 2013 week 8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SEA(a)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> @ STL(h) 2013 week 8</t>
     </r>
   </si>
 </sst>
@@ -3101,7 +3122,7 @@
       </c>
       <c r="B2">
         <f>'Week 4 results'!B2+'Week 5 results'!B2+'Week 6 results'!B2+'Week 7 results'!B2+'Week 8 results'!B2</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C2">
         <f>'Week 4 results'!C2+'Week 5 results'!C2+'Week 6 results'!C2+'Week 7 results'!C2+'Week 8 results'!C2</f>
@@ -3113,15 +3134,15 @@
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E7" si="0">B2+C2+D2</f>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F2" s="14">
         <f t="shared" ref="F2:F7" si="1">B2/(E2-D2)</f>
-        <v>0.59649122807017541</v>
+        <v>0.60344827586206895</v>
       </c>
       <c r="G2" s="14">
         <f t="shared" ref="G2:G7" si="2">B2/E2</f>
-        <v>0.58620689655172409</v>
+        <v>0.59322033898305082</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -3130,7 +3151,7 @@
       </c>
       <c r="B3">
         <f>'Week 4 results'!B3+'Week 5 results'!B3+'Week 6 results'!B3+'Week 7 results'!B3+'Week 8 results'!B3</f>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C3">
         <f>'Week 4 results'!C3+'Week 5 results'!C3+'Week 6 results'!C3+'Week 7 results'!C3+'Week 8 results'!C3</f>
@@ -3142,15 +3163,15 @@
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F3" s="14">
         <f t="shared" si="1"/>
-        <v>0.63636363636363635</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="G3" s="14">
         <f t="shared" si="2"/>
-        <v>0.60344827586206895</v>
+        <v>0.61016949152542377</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -3159,7 +3180,7 @@
       </c>
       <c r="B4">
         <f>'Week 4 results'!B4+'Week 5 results'!B4+'Week 6 results'!B4+'Week 7 results'!B4+'Week 8 results'!B4</f>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C4">
         <f>'Week 4 results'!C4+'Week 5 results'!C4+'Week 6 results'!C4+'Week 7 results'!C4+'Week 8 results'!C4</f>
@@ -3171,15 +3192,15 @@
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F4" s="14">
         <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
+        <v>0.67241379310344829</v>
       </c>
       <c r="G4" s="14">
         <f t="shared" si="2"/>
-        <v>0.65517241379310343</v>
+        <v>0.66101694915254239</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -3188,7 +3209,7 @@
       </c>
       <c r="B5">
         <f>'Week 4 results'!B5+'Week 5 results'!B5+'Week 6 results'!B5+'Week 7 results'!B5+'Week 8 results'!B5</f>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C5">
         <f>'Week 4 results'!C5+'Week 5 results'!C5+'Week 6 results'!C5+'Week 7 results'!C5+'Week 8 results'!C5</f>
@@ -3200,15 +3221,15 @@
       </c>
       <c r="E5">
         <f>B5+C5+D5</f>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F5" s="14">
         <f t="shared" si="1"/>
-        <v>0.68627450980392157</v>
+        <v>0.69230769230769229</v>
       </c>
       <c r="G5" s="14">
         <f t="shared" si="2"/>
-        <v>0.60344827586206895</v>
+        <v>0.61016949152542377</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -3217,7 +3238,7 @@
       </c>
       <c r="B6">
         <f>'Week 4 results'!B6+'Week 5 results'!B6+'Week 6 results'!B6+'Week 7 results'!B6+'Week 8 results'!B6</f>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6">
         <f>'Week 4 results'!C6+'Week 5 results'!C6+'Week 6 results'!C6+'Week 7 results'!C6+'Week 8 results'!C6</f>
@@ -3229,15 +3250,15 @@
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F6" s="14">
         <f t="shared" si="1"/>
-        <v>0.61111111111111116</v>
+        <v>0.61818181818181817</v>
       </c>
       <c r="G6" s="14">
         <f t="shared" si="2"/>
-        <v>0.56896551724137934</v>
+        <v>0.57627118644067798</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -3246,7 +3267,7 @@
       </c>
       <c r="B7">
         <f>'Week 4 results'!B7+'Week 5 results'!B7+'Week 6 results'!B7+'Week 7 results'!B7+'Week 8 results'!B7</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7">
         <f>'Week 4 results'!C7+'Week 5 results'!C7+'Week 6 results'!C7+'Week 7 results'!C7+'Week 8 results'!C7</f>
@@ -3258,15 +3279,15 @@
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F7" s="14">
         <f t="shared" si="1"/>
-        <v>0.59649122807017541</v>
+        <v>0.60344827586206895</v>
       </c>
       <c r="G7" s="14">
         <f t="shared" si="2"/>
-        <v>0.58620689655172409</v>
+        <v>0.59322033898305082</v>
       </c>
     </row>
   </sheetData>
@@ -4745,7 +4766,7 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4770,43 +4791,43 @@
         <v>187</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F1" s="16" t="s">
+        <v>390</v>
+      </c>
+      <c r="G1" s="16" t="s">
         <v>391</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="16" t="s">
         <v>392</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="I1" s="16" t="s">
         <v>393</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="J1" s="16" t="s">
         <v>394</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="K1" s="16" t="s">
         <v>395</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="L1" s="16" t="s">
         <v>396</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="M1" s="16" t="s">
         <v>397</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="N1" s="16" t="s">
         <v>398</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="O1" s="16" t="s">
         <v>399</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="P1" s="16" t="s">
         <v>400</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="Q1" s="16" t="s">
         <v>401</v>
-      </c>
-      <c r="Q1" s="16" t="s">
-        <v>318</v>
       </c>
       <c r="R1" s="16"/>
     </row>
@@ -4815,7 +4836,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -4824,43 +4845,43 @@
         <v>0</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>343</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="G2" s="7" t="s">
         <v>344</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="I2" s="7" t="s">
         <v>346</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="12" t="s">
         <v>347</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="K2" s="7" t="s">
         <v>348</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>349</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="M2" s="7" t="s">
         <v>350</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="N2" s="7" t="s">
         <v>351</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>352</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>275</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>342</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>353</v>
+        <v>341</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -4868,7 +4889,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -4877,43 +4898,43 @@
         <v>0</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="G3" s="7" t="s">
         <v>332</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="12" t="s">
         <v>333</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="I3" s="7" t="s">
         <v>334</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>335</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="L3" s="12" t="s">
         <v>337</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="M3" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>339</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="O3" s="12" t="s">
         <v>340</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>341</v>
       </c>
       <c r="P3" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="Q3" t="s">
-        <v>342</v>
+      <c r="Q3" s="7" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -4921,7 +4942,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -4930,43 +4951,43 @@
         <v>0</v>
       </c>
       <c r="E4" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="F4" s="12" t="s">
         <v>319</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>320</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>72</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>231</v>
       </c>
       <c r="J4" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="K4" s="7" t="s">
         <v>322</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="L4" s="12" t="s">
         <v>323</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="M4" s="7" t="s">
         <v>324</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="N4" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="O4" s="12" t="s">
         <v>326</v>
       </c>
-      <c r="O4" s="12" t="s">
+      <c r="P4" s="7" t="s">
         <v>327</v>
       </c>
-      <c r="P4" s="7" t="s">
+      <c r="Q4" s="7" t="s">
         <v>328</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -4974,7 +4995,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -4983,43 +5004,43 @@
         <v>1</v>
       </c>
       <c r="E5" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>354</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="G5" s="7" t="s">
         <v>355</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="H5" s="10" t="s">
         <v>356</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="I5" s="7" t="s">
         <v>357</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="J5" s="7" t="s">
         <v>358</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>359</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>265</v>
       </c>
       <c r="L5" s="12" t="s">
+        <v>359</v>
+      </c>
+      <c r="M5" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="N5" s="7" t="s">
         <v>361</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="O5" s="12" t="s">
         <v>362</v>
       </c>
-      <c r="O5" s="12" t="s">
+      <c r="P5" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="P5" s="7" t="s">
+      <c r="Q5" s="7" t="s">
         <v>364</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -5027,7 +5048,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -5036,43 +5057,43 @@
         <v>0</v>
       </c>
       <c r="E6" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>366</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="G6" s="7" t="s">
         <v>367</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="12" t="s">
         <v>368</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="I6" s="7" t="s">
         <v>369</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="J6" s="7" t="s">
         <v>370</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="K6" s="7" t="s">
         <v>371</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="L6" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="M6" s="7" t="s">
         <v>372</v>
       </c>
-      <c r="L6" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="M6" s="7" t="s">
+      <c r="N6" s="7" t="s">
         <v>373</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="O6" s="12" t="s">
         <v>374</v>
       </c>
-      <c r="O6" s="12" t="s">
+      <c r="P6" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="P6" s="7" t="s">
+      <c r="Q6" s="7" t="s">
         <v>376</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -5080,7 +5101,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -5089,43 +5110,43 @@
         <v>0</v>
       </c>
       <c r="E7" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="F7" s="12" t="s">
         <v>378</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="G7" s="7" t="s">
         <v>379</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="H7" s="12" t="s">
         <v>380</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="I7" s="7" t="s">
         <v>381</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="J7" s="12" t="s">
         <v>382</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="K7" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="L7" s="7" t="s">
         <v>384</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="M7" s="7" t="s">
         <v>385</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="N7" s="7" t="s">
         <v>386</v>
       </c>
-      <c r="N7" s="7" t="s">
+      <c r="O7" s="12" t="s">
         <v>387</v>
       </c>
-      <c r="O7" s="12" t="s">
+      <c r="P7" s="7" t="s">
         <v>388</v>
       </c>
-      <c r="P7" s="7" t="s">
+      <c r="Q7" s="7" t="s">
         <v>389</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Week 9 testing spreadsheet update
</commit_message>
<xml_diff>
--- a/AFootball testing results.xlsx
+++ b/AFootball testing results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Season results" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="Week 6 results" sheetId="4" r:id="rId4"/>
     <sheet name="Week 7 results" sheetId="5" r:id="rId5"/>
     <sheet name="Week 8 results" sheetId="6" r:id="rId6"/>
+    <sheet name="Week 9 results" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="424">
   <si>
     <t>AF613_logsig base randomized w&amp;b*</t>
   </si>
@@ -2569,6 +2570,72 @@
       </rPr>
       <t xml:space="preserve"> @ STL(h) 2013 week 8</t>
     </r>
+  </si>
+  <si>
+    <t>CIN(a) @ MIA(h) 2013 Week 9</t>
+  </si>
+  <si>
+    <t>ATL(a) @ CAR(h) 2013 Week 9</t>
+  </si>
+  <si>
+    <t>SD(a) @ WAS(h) 2013 Week 9</t>
+  </si>
+  <si>
+    <t>NO(a) @ NYJ(h) 2013 Week 9</t>
+  </si>
+  <si>
+    <t>TEN(a) @ STL(h) 2013 Week 9</t>
+  </si>
+  <si>
+    <t>MIN(a) @ DAL(h) 2013 Week 9</t>
+  </si>
+  <si>
+    <t>KC(a) @ BUF(h) 2013 Week 9</t>
+  </si>
+  <si>
+    <t>TB(a) @ SEA(h) 2013 Week 9</t>
+  </si>
+  <si>
+    <t>PHI(a) @ OAK(h) 2013 Week 9</t>
+  </si>
+  <si>
+    <t>PIT(a) @ NE(h) 2013 Week 9</t>
+  </si>
+  <si>
+    <t>BAL(a) @ CLE(h) 2013 Week 9</t>
+  </si>
+  <si>
+    <t>IND(a) @ HOU(h) 2013 Week 9</t>
+  </si>
+  <si>
+    <t>CHI(a) @ GB(h) 2013 Week 9</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9957 / ON002(away win): 0.0042</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.0075 / ON002(away win): 0.9924</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9844 / ON002(away win): 0.0155</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.0007 / ON002(away win): 0.9992</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.1170 / ON002(away win): 0.8829</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.6642 / ON002(away win): 0.3357</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.1681 / ON002(away win): 0.8318</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.8275 / ON002(away win): 0.1724</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.9985 / ON002(away win): 0.0014</t>
   </si>
 </sst>
 </file>
@@ -3079,8 +3146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3121,15 +3188,15 @@
         <v>223</v>
       </c>
       <c r="B2">
-        <f>'Week 4 results'!B2+'Week 5 results'!B2+'Week 6 results'!B2+'Week 7 results'!B2+'Week 8 results'!B2</f>
+        <f>'Week 4 results'!B2+'Week 5 results'!B2+'Week 6 results'!B2+'Week 7 results'!B2+'Week 8 results'!B2+'Week 9 results'!B2</f>
         <v>35</v>
       </c>
       <c r="C2">
-        <f>'Week 4 results'!C2+'Week 5 results'!C2+'Week 6 results'!C2+'Week 7 results'!C2+'Week 8 results'!C2</f>
+        <f>'Week 4 results'!C2+'Week 5 results'!C2+'Week 6 results'!C2+'Week 7 results'!C2+'Week 8 results'!C2+'Week 9 results'!C2</f>
         <v>23</v>
       </c>
       <c r="D2">
-        <f>'Week 4 results'!D2+'Week 5 results'!D2+'Week 6 results'!D2+'Week 7 results'!D2+'Week 8 results'!D2</f>
+        <f>'Week 4 results'!D2+'Week 5 results'!D2+'Week 6 results'!D2+'Week 7 results'!D2+'Week 8 results'!D2+'Week 9 results'!D2</f>
         <v>1</v>
       </c>
       <c r="E2">
@@ -3150,15 +3217,15 @@
         <v>222</v>
       </c>
       <c r="B3">
-        <f>'Week 4 results'!B3+'Week 5 results'!B3+'Week 6 results'!B3+'Week 7 results'!B3+'Week 8 results'!B3</f>
+        <f>'Week 4 results'!B3+'Week 5 results'!B3+'Week 6 results'!B3+'Week 7 results'!B3+'Week 8 results'!B3+'Week 9 results'!B3</f>
         <v>36</v>
       </c>
       <c r="C3">
-        <f>'Week 4 results'!C3+'Week 5 results'!C3+'Week 6 results'!C3+'Week 7 results'!C3+'Week 8 results'!C3</f>
+        <f>'Week 4 results'!C3+'Week 5 results'!C3+'Week 6 results'!C3+'Week 7 results'!C3+'Week 8 results'!C3+'Week 9 results'!C3</f>
         <v>20</v>
       </c>
       <c r="D3">
-        <f>'Week 4 results'!D3+'Week 5 results'!D3+'Week 6 results'!D3+'Week 7 results'!D3+'Week 8 results'!D3</f>
+        <f>'Week 4 results'!D3+'Week 5 results'!D3+'Week 6 results'!D3+'Week 7 results'!D3+'Week 8 results'!D3+'Week 9 results'!D3</f>
         <v>3</v>
       </c>
       <c r="E3">
@@ -3179,15 +3246,15 @@
         <v>221</v>
       </c>
       <c r="B4">
-        <f>'Week 4 results'!B4+'Week 5 results'!B4+'Week 6 results'!B4+'Week 7 results'!B4+'Week 8 results'!B4</f>
+        <f>'Week 4 results'!B4+'Week 5 results'!B4+'Week 6 results'!B4+'Week 7 results'!B4+'Week 8 results'!B4+'Week 9 results'!B4</f>
         <v>39</v>
       </c>
       <c r="C4">
-        <f>'Week 4 results'!C4+'Week 5 results'!C4+'Week 6 results'!C4+'Week 7 results'!C4+'Week 8 results'!C4</f>
+        <f>'Week 4 results'!C4+'Week 5 results'!C4+'Week 6 results'!C4+'Week 7 results'!C4+'Week 8 results'!C4+'Week 9 results'!C4</f>
         <v>19</v>
       </c>
       <c r="D4">
-        <f>'Week 4 results'!D4+'Week 5 results'!D4+'Week 6 results'!D4+'Week 7 results'!D4+'Week 8 results'!D4</f>
+        <f>'Week 4 results'!D4+'Week 5 results'!D4+'Week 6 results'!D4+'Week 7 results'!D4+'Week 8 results'!D4+'Week 9 results'!D4</f>
         <v>1</v>
       </c>
       <c r="E4">
@@ -3208,15 +3275,15 @@
         <v>220</v>
       </c>
       <c r="B5">
-        <f>'Week 4 results'!B5+'Week 5 results'!B5+'Week 6 results'!B5+'Week 7 results'!B5+'Week 8 results'!B5</f>
+        <f>'Week 4 results'!B5+'Week 5 results'!B5+'Week 6 results'!B5+'Week 7 results'!B5+'Week 8 results'!B5+'Week 9 results'!B5</f>
         <v>36</v>
       </c>
       <c r="C5">
-        <f>'Week 4 results'!C5+'Week 5 results'!C5+'Week 6 results'!C5+'Week 7 results'!C5+'Week 8 results'!C5</f>
+        <f>'Week 4 results'!C5+'Week 5 results'!C5+'Week 6 results'!C5+'Week 7 results'!C5+'Week 8 results'!C5+'Week 9 results'!C5</f>
         <v>16</v>
       </c>
       <c r="D5">
-        <f>'Week 4 results'!D5+'Week 5 results'!D5+'Week 6 results'!D5+'Week 7 results'!D5+'Week 8 results'!D5</f>
+        <f>'Week 4 results'!D5+'Week 5 results'!D5+'Week 6 results'!D5+'Week 7 results'!D5+'Week 8 results'!D5+'Week 9 results'!D5</f>
         <v>7</v>
       </c>
       <c r="E5">
@@ -3237,15 +3304,15 @@
         <v>219</v>
       </c>
       <c r="B6">
-        <f>'Week 4 results'!B6+'Week 5 results'!B6+'Week 6 results'!B6+'Week 7 results'!B6+'Week 8 results'!B6</f>
+        <f>'Week 4 results'!B6+'Week 5 results'!B6+'Week 6 results'!B6+'Week 7 results'!B6+'Week 8 results'!B6+'Week 9 results'!B6</f>
         <v>34</v>
       </c>
       <c r="C6">
-        <f>'Week 4 results'!C6+'Week 5 results'!C6+'Week 6 results'!C6+'Week 7 results'!C6+'Week 8 results'!C6</f>
+        <f>'Week 4 results'!C6+'Week 5 results'!C6+'Week 6 results'!C6+'Week 7 results'!C6+'Week 8 results'!C6+'Week 9 results'!C6</f>
         <v>21</v>
       </c>
       <c r="D6">
-        <f>'Week 4 results'!D6+'Week 5 results'!D6+'Week 6 results'!D6+'Week 7 results'!D6+'Week 8 results'!D6</f>
+        <f>'Week 4 results'!D6+'Week 5 results'!D6+'Week 6 results'!D6+'Week 7 results'!D6+'Week 8 results'!D6+'Week 9 results'!D6</f>
         <v>4</v>
       </c>
       <c r="E6">
@@ -3266,15 +3333,15 @@
         <v>218</v>
       </c>
       <c r="B7">
-        <f>'Week 4 results'!B7+'Week 5 results'!B7+'Week 6 results'!B7+'Week 7 results'!B7+'Week 8 results'!B7</f>
+        <f>'Week 4 results'!B7+'Week 5 results'!B7+'Week 6 results'!B7+'Week 7 results'!B7+'Week 8 results'!B7+'Week 9 results'!B7</f>
         <v>35</v>
       </c>
       <c r="C7">
-        <f>'Week 4 results'!C7+'Week 5 results'!C7+'Week 6 results'!C7+'Week 7 results'!C7+'Week 8 results'!C7</f>
+        <f>'Week 4 results'!C7+'Week 5 results'!C7+'Week 6 results'!C7+'Week 7 results'!C7+'Week 8 results'!C7+'Week 9 results'!C7</f>
         <v>23</v>
       </c>
       <c r="D7">
-        <f>'Week 4 results'!D7+'Week 5 results'!D7+'Week 6 results'!D7+'Week 7 results'!D7+'Week 8 results'!D7</f>
+        <f>'Week 4 results'!D7+'Week 5 results'!D7+'Week 6 results'!D7+'Week 7 results'!D7+'Week 8 results'!D7+'Week 9 results'!D7</f>
         <v>1</v>
       </c>
       <c r="E7">
@@ -4766,7 +4833,7 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5153,4 +5220,146 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Q7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="5" max="17" width="51.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="4" customFormat="1">
+      <c r="A1" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>327</v>
+      </c>
+      <c r="F4" t="s">
+        <v>415</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" t="s">
+        <v>157</v>
+      </c>
+      <c r="I4" t="s">
+        <v>416</v>
+      </c>
+      <c r="J4" t="s">
+        <v>417</v>
+      </c>
+      <c r="K4" t="s">
+        <v>418</v>
+      </c>
+      <c r="L4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" t="s">
+        <v>419</v>
+      </c>
+      <c r="N4" t="s">
+        <v>420</v>
+      </c>
+      <c r="O4" t="s">
+        <v>421</v>
+      </c>
+      <c r="P4" t="s">
+        <v>422</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
testing results spreadsheet update week 11
</commit_message>
<xml_diff>
--- a/AFootball testing results.xlsx
+++ b/AFootball testing results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Season results" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="473">
   <si>
     <t>AF613_logsig base randomized w&amp;b*</t>
   </si>
@@ -3340,6 +3340,69 @@
   </si>
   <si>
     <t>ON001(home win): 0.19930 / ON002(away win): 0.80069</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (a) @  (h) 2013 Week 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (a) @  (h) 2013 Week 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (a) @  (h) 2013 Week 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (a) @  (h) 2013 Week 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (a) @  (h) 2013 Week 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (a) @  (h) 2013 Week 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> IND(a) @ TEN(h) 2013 Week 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NYJ(a) @ BUF(h) 2013 Week 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BAL(a) @ CHI(h) 2013 Week 11</t>
+  </si>
+  <si>
+    <t>CLE(a) @ CIN(h) 2013 Week 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DET(a) @ PIT(h) 2013 Week 11</t>
+  </si>
+  <si>
+    <t>OAK(a) @ HOU(h) 2013 Week 11</t>
+  </si>
+  <si>
+    <t>ARI(a) @ JAC(h) 2013 Week 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> WAS(a) @ PHI(h) 2013 Week 11</t>
+  </si>
+  <si>
+    <t>ATL(a) @ TB(h) 2013 Week 11</t>
+  </si>
+  <si>
+    <t>SD(a) @ MIA(h) 2013 Week 11</t>
+  </si>
+  <si>
+    <t>MIN(a) @ SEA(h) 2013 Week 11</t>
+  </si>
+  <si>
+    <t>SF(a) @ NO(h) 2013 Week 11</t>
+  </si>
+  <si>
+    <t>KC(a) @ DEN(h) 2013 Week 11</t>
+  </si>
+  <si>
+    <t>NE(a) @ CAR(h) 2013 Week 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GB(a) @ NYG(h) 2013 Week 11</t>
   </si>
 </sst>
 </file>
@@ -3850,8 +3913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3950,15 +4013,15 @@
         <v>221</v>
       </c>
       <c r="B4">
-        <f>'Week 4 results'!B4+'Week 5 results'!B4+'Week 6 results'!B4+'Week 7 results'!B4+'Week 8 results'!B4+'Week 9 results'!B4+'Week 10 results'!B4</f>
+        <f>'Week 4 results'!B4+'Week 5 results'!B4+'Week 6 results'!B4+'Week 7 results'!B4+'Week 8 results'!B4+'Week 9 results'!B4+'Week 10 results'!B4+'Week 11 results'!B4+'Week 12 results'!B4+'Week 13 results'!B4+'Week 14 results'!B4+'Week 15 results'!B4+'Week 16 results'!B4+'Week 17 results'!B4</f>
         <v>52</v>
       </c>
       <c r="C4">
-        <f>'Week 4 results'!C4+'Week 5 results'!C4+'Week 6 results'!C4+'Week 7 results'!C4+'Week 8 results'!C4+'Week 9 results'!C4+'Week 10 results'!C4</f>
+        <f>'Week 4 results'!C4+'Week 5 results'!C4+'Week 6 results'!C4+'Week 7 results'!C4+'Week 8 results'!C4+'Week 9 results'!C4+'Week 10 results'!C4+'Week 11 results'!C4+'Week 12 results'!C4+'Week 13 results'!C4+'Week 14 results'!C4+'Week 15 results'!C4+'Week 16 results'!C4+'Week 17 results'!C4</f>
         <v>33</v>
       </c>
       <c r="D4">
-        <f>'Week 4 results'!D4+'Week 5 results'!D4+'Week 6 results'!D4+'Week 7 results'!D4+'Week 8 results'!D4+'Week 9 results'!D4+'Week 10 results'!D4</f>
+        <f>'Week 4 results'!D4+'Week 5 results'!D4+'Week 6 results'!D4+'Week 7 results'!D4+'Week 8 results'!D4+'Week 9 results'!D4+'Week 10 results'!D4+'Week 11 results'!D4+'Week 12 results'!D4+'Week 13 results'!D4+'Week 14 results'!D4+'Week 15 results'!D4+'Week 16 results'!D4+'Week 17 results'!D4</f>
         <v>1</v>
       </c>
       <c r="E4">
@@ -4069,48 +4132,62 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="2" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="51.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:5" s="4" customFormat="1">
       <c r="A1" s="16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -4122,48 +4199,62 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="2" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="51.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:5" s="4" customFormat="1">
       <c r="A1" s="16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -4175,48 +4266,62 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="2" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="51.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:5" s="4" customFormat="1">
       <c r="A1" s="16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -4228,48 +4333,62 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="2" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="51.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:5" s="4" customFormat="1">
       <c r="A1" s="16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -4281,48 +4400,62 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="2" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="51.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:5" s="4" customFormat="1">
       <c r="A1" s="16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -4334,48 +4467,62 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="2" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="51.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:5" s="4" customFormat="1">
       <c r="A1" s="16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -6400,7 +6547,7 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6554,53 +6701,122 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="2" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="19" width="51.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:19" s="4" customFormat="1">
       <c r="A1" s="16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>458</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>469</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:19">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
week 13 testing results + week 14 data set
</commit_message>
<xml_diff>
--- a/AFootball testing results.xlsx
+++ b/AFootball testing results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="6" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Season results" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="547">
   <si>
     <t>AF613_logsig base randomized w&amp;b*</t>
   </si>
@@ -4216,52 +4216,466 @@
     <t>ON001(home win): 0.05776  / ON002(away win): 0.94223</t>
   </si>
   <si>
-    <t xml:space="preserve"> GB(a) @  DET(h) 2013 Week 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> OAK(a) @  DAL(h) 2013 Week 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> PIT(a) @  BAL(h) 2013 Week 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> JAC(a) @  CLE(h) 2013 Week 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> TB(a) @  CAR(h) 2013 Week 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CHI(a) @  MIN(h) 2013 Week 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> NE(a) @  HOU(h) 2013 Week 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> TEN(a) @  IND(h) 2013 Week 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> MIA(a) @  NYJ(h) 2013 Week 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ARI(a) @  PHI(h) 2013 Week 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ATL(a) @  BUF(h) 2013 Week 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> STL(a) @  SF(h) 2013 Week 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CIN(a) @  SD(h) 2013 Week 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DEN(a) @  KC(h) 2013 Week 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> NYG(a) @  WAS(h) 2013 Week 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> NO(a) @  SEA(h) 2013 Week 13</t>
+    <r>
+      <t xml:space="preserve"> GB(a) @  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DET(h)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2013 Week 13</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> OAK(a) @  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DAL(h)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2013 Week 13</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> PIT(a) @  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BAL(h)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2013 Week 13</t>
+    </r>
+  </si>
+  <si>
+    <t>ON001(home win): 0.01048  / ON002(away win): 0.98951</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.77181  / ON002(away win): 0.22818</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.02471  / ON002(away win): 0.97528</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> JAC(a)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> @  CLE(h) 2013 Week 13</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> TB(a) @  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CAR(h)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2013 Week 13</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> CHI(a) @  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MIN(h)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2013 Week 13</t>
+    </r>
+  </si>
+  <si>
+    <t>ON001(home win): 0.94474  / ON002(away win): 0.05525</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.99916  / ON002(away win): 0.00083</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.09735  / ON002(away win): 0.90264</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> NE(a) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@  HOU(h) 2013 Week 13</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> TEN(a) @ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> IND(h)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2013 Week 13</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> MIA(a)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> @  NYJ(h) 2013 Week 13</t>
+    </r>
+  </si>
+  <si>
+    <t>ON001(home win): 0.27019  / ON002(away win): 0.72980</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.00310  / ON002(away win): 0.99689</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.01673  / ON002(away win): 0.98326</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> ARI(a) @  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PHI(h)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2013 Week 13</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ATL(a)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> @  BUF(h) 2013 Week 13</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> STL(a) @  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">SF(h) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2013 Week 13</t>
+    </r>
+  </si>
+  <si>
+    <t>ON001(home win): 0.06872  / ON002(away win): 0.93127</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.77306  / ON002(away win): 0.22693</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.93843  / ON002(away win): 0.06156</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> CIN(a)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> @  SD(h) 2013 Week 13</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> DEN(a)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  @  KC(h) 2013 Week 13</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NYG(a)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> @  WAS(h) 2013 Week 13</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> NO(a) @  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SEA(h)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2013 Week 13</t>
+    </r>
+  </si>
+  <si>
+    <t>ON001(home win): 0.02261  / ON002(away win): 0.97738</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.03083  / ON002(away win): 0.96916</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.97207  / ON002(away win): 0.02792</t>
+  </si>
+  <si>
+    <t>ON001(home win): 0.00486  / ON002(away win): 0.99513</t>
   </si>
 </sst>
 </file>
@@ -4772,8 +5186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4873,11 +5287,11 @@
       </c>
       <c r="B4">
         <f>'Week 4 results'!B4+'Week 5 results'!B4+'Week 6 results'!B4+'Week 7 results'!B4+'Week 8 results'!B4+'Week 9 results'!B4+'Week 10 results'!B4+'Week 11 results'!B4+'Week 12 results'!B4+'Week 13 results'!B4+'Week 14 results'!B4+'Week 15 results'!B4+'Week 16 results'!B4+'Week 17 results'!B4</f>
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="C4">
         <f>'Week 4 results'!C4+'Week 5 results'!C4+'Week 6 results'!C4+'Week 7 results'!C4+'Week 8 results'!C4+'Week 9 results'!C4+'Week 10 results'!C4+'Week 11 results'!C4+'Week 12 results'!C4+'Week 13 results'!C4+'Week 14 results'!C4+'Week 15 results'!C4+'Week 16 results'!C4+'Week 17 results'!C4</f>
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="D4">
         <f>'Week 4 results'!D4+'Week 5 results'!D4+'Week 6 results'!D4+'Week 7 results'!D4+'Week 8 results'!D4+'Week 9 results'!D4+'Week 10 results'!D4+'Week 11 results'!D4+'Week 12 results'!D4+'Week 13 results'!D4+'Week 14 results'!D4+'Week 15 results'!D4+'Week 16 results'!D4+'Week 17 results'!D4</f>
@@ -4885,15 +5299,15 @@
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="F4" s="14">
         <f t="shared" si="1"/>
-        <v>0.6228070175438597</v>
+        <v>0.6</v>
       </c>
       <c r="G4" s="14">
         <f t="shared" si="2"/>
-        <v>0.61739130434782608</v>
+        <v>0.59541984732824427</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -5148,8 +5562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5182,43 +5596,43 @@
         <v>517</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>521</v>
+        <v>527</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>522</v>
+        <v>528</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>523</v>
+        <v>529</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>524</v>
+        <v>533</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>525</v>
+        <v>534</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>526</v>
+        <v>535</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>527</v>
+        <v>539</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>528</v>
+        <v>540</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>529</v>
+        <v>541</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>530</v>
+        <v>542</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -5235,53 +5649,59 @@
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
-        <v>456</v>
-      </c>
-      <c r="F4" t="s">
-        <v>456</v>
-      </c>
-      <c r="G4" t="s">
-        <v>456</v>
-      </c>
-      <c r="H4" t="s">
-        <v>456</v>
-      </c>
-      <c r="I4" t="s">
-        <v>456</v>
-      </c>
-      <c r="J4" t="s">
-        <v>456</v>
-      </c>
-      <c r="K4" t="s">
-        <v>456</v>
-      </c>
-      <c r="L4" t="s">
-        <v>456</v>
-      </c>
-      <c r="M4" t="s">
-        <v>456</v>
-      </c>
-      <c r="N4" t="s">
-        <v>456</v>
-      </c>
-      <c r="O4" t="s">
-        <v>456</v>
-      </c>
-      <c r="P4" t="s">
-        <v>456</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>456</v>
-      </c>
-      <c r="R4" t="s">
-        <v>456</v>
-      </c>
-      <c r="S4" t="s">
-        <v>456</v>
-      </c>
-      <c r="T4" t="s">
-        <v>456</v>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>518</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>520</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>524</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>525</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>526</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>531</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>532</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>536</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>537</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>538</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>543</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>544</v>
+      </c>
+      <c r="S4" s="12" t="s">
+        <v>545</v>
+      </c>
+      <c r="T4" s="12" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -5301,6 +5721,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5308,15 +5729,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
     <col min="2" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="51.7109375" customWidth="1"/>
+    <col min="5" max="20" width="51.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1">

</xml_diff>